<commit_message>
readme updated, notebooks added
</commit_message>
<xml_diff>
--- a/dataset/reproducibility_studies_metadata.xlsx
+++ b/dataset/reproducibility_studies_metadata.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olddominion-my.sharepoint.com/personal/oruma001_odu_edu/Documents/Lemos_OneDrive_odu_windows/Research_ODU/R001_Fall_2023_AI_Reproducibility/github/cc25k-citation-contexts-for-ai-reproducibility/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{8F1F9050-CA5C-4530-9CCA-3C8A45094DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AA0CC0F-002C-48A7-9605-21A21300EE6A}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-3375" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-3375" windowWidth="29040" windowHeight="15840" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -4977,13 +4977,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -4994,7 +5000,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <u val="single"/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -5010,7 +5016,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.399980008602142"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5036,27 +5042,56 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
+  <cellStyleXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
+      <alignment/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="20" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -5116,6 +5151,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -5413,33 +5516,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0" topLeftCell="A1">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="X1" sqref="X1:AC1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.7142857142857" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="9" width="25.7109375" customWidth="1"/>
-    <col min="10" max="10" width="44.85546875" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="41.42578125" customWidth="1"/>
-    <col min="13" max="13" width="39.140625" customWidth="1"/>
-    <col min="14" max="14" width="27.5703125" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.8571428571429" customWidth="1"/>
+    <col min="5" max="9" width="25.7142857142857" customWidth="1"/>
+    <col min="10" max="10" width="44.8571428571429" customWidth="1"/>
+    <col min="11" max="11" width="25.7142857142857" customWidth="1"/>
+    <col min="12" max="12" width="41.4285714285714" customWidth="1"/>
+    <col min="13" max="13" width="39.1428571428571" customWidth="1"/>
+    <col min="14" max="14" width="27.5714285714286" customWidth="1"/>
+    <col min="15" max="15" width="31.1428571428571" customWidth="1"/>
     <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="21.5703125" customWidth="1"/>
-    <col min="18" max="23" width="25.7109375" customWidth="1"/>
+    <col min="17" max="17" width="21.5714285714286" customWidth="1"/>
+    <col min="18" max="23" width="25.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5510,7 +5614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -5563,7 +5667,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -5616,7 +5720,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -5669,7 +5773,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="15" customHeight="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -5722,7 +5826,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="15" customHeight="1">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -5775,7 +5879,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="15" customHeight="1">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -5828,7 +5932,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="15" customHeight="1">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -5881,7 +5985,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="15" customHeight="1">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -5934,7 +6038,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="15" customHeight="1">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -5987,7 +6091,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="15" customHeight="1">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -6040,7 +6144,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="15" customHeight="1">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -6093,7 +6197,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -6146,7 +6250,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="15" customHeight="1">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -6199,7 +6303,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="15" customHeight="1">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -6252,7 +6356,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="15" customHeight="1">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -6305,7 +6409,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="15" customHeight="1">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -6358,7 +6462,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="15" customHeight="1">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -6411,7 +6515,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="15" customHeight="1">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -6464,7 +6568,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="15" customHeight="1">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -6517,7 +6621,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="15" customHeight="1">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -6570,7 +6674,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="15" customHeight="1">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -6623,7 +6727,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="15" customHeight="1">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -6676,7 +6780,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="15" customHeight="1">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -6729,7 +6833,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="15" customHeight="1">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -6782,7 +6886,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="15" customHeight="1">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -6835,7 +6939,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="15" customHeight="1">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -6888,7 +6992,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="15" customHeight="1">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -6941,7 +7045,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="15" customHeight="1">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -6994,7 +7098,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="15" customHeight="1">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -7047,7 +7151,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="15" customHeight="1">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -7100,7 +7204,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="15" customHeight="1">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -7153,7 +7257,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="15" customHeight="1">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -7206,7 +7310,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="15" customHeight="1">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -7259,7 +7363,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="15" customHeight="1">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -7312,7 +7416,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="15" customHeight="1">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -7365,7 +7469,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="37" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="15" customHeight="1">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -7418,7 +7522,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="15" customHeight="1">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -7471,7 +7575,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="15" customHeight="1">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -7524,7 +7628,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="40" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="15" customHeight="1">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -7577,7 +7681,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="15" customHeight="1">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -7630,7 +7734,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="42" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="15" customHeight="1">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -7683,7 +7787,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="15" customHeight="1">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -7736,7 +7840,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="15" customHeight="1">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -7789,7 +7893,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="15" customHeight="1">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -7842,7 +7946,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="15" customHeight="1">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -7895,7 +7999,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="15" customHeight="1">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -7957,7 +8061,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="15" customHeight="1">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -8025,7 +8129,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="15" customHeight="1">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -8096,7 +8200,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="15" customHeight="1">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -8164,7 +8268,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="15" customHeight="1">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -8232,7 +8336,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="15" customHeight="1">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -8303,7 +8407,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="15" customHeight="1">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -8374,7 +8478,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="15" customHeight="1">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -8442,7 +8546,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="55" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="15" customHeight="1">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -8510,7 +8614,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="15" customHeight="1">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -8581,7 +8685,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="15" customHeight="1">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -8652,7 +8756,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="15" customHeight="1">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -8720,7 +8824,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" ht="15" customHeight="1">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -8788,7 +8892,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" ht="15" customHeight="1">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -8859,7 +8963,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" ht="15" customHeight="1">
       <c r="A61" t="s">
         <v>80</v>
       </c>
@@ -8927,7 +9031,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" ht="15" customHeight="1">
       <c r="A62" t="s">
         <v>81</v>
       </c>
@@ -8998,7 +9102,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="15" customHeight="1">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -9069,7 +9173,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" ht="15" customHeight="1">
       <c r="A64" t="s">
         <v>83</v>
       </c>
@@ -9140,7 +9244,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" ht="15" customHeight="1">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -9211,7 +9315,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="66" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" ht="15" customHeight="1">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -9279,7 +9383,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" ht="15" customHeight="1">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -9347,7 +9451,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="68" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" ht="15" customHeight="1">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -9415,7 +9519,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" ht="15" customHeight="1">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -9486,7 +9590,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" ht="15" customHeight="1">
       <c r="A70" t="s">
         <v>89</v>
       </c>
@@ -9554,7 +9658,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="71" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" ht="15" customHeight="1">
       <c r="A71" t="s">
         <v>90</v>
       </c>
@@ -9622,7 +9726,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" ht="15" customHeight="1">
       <c r="A72" t="s">
         <v>91</v>
       </c>
@@ -9690,7 +9794,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="73" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" ht="15" customHeight="1">
       <c r="A73" t="s">
         <v>92</v>
       </c>
@@ -9761,7 +9865,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="74" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" ht="15" customHeight="1">
       <c r="A74" t="s">
         <v>93</v>
       </c>
@@ -9829,7 +9933,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="75" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" ht="15" customHeight="1">
       <c r="A75" t="s">
         <v>94</v>
       </c>
@@ -9900,7 +10004,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" ht="15" customHeight="1">
       <c r="A76" t="s">
         <v>95</v>
       </c>
@@ -9968,7 +10072,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" ht="15" customHeight="1">
       <c r="A77" t="s">
         <v>96</v>
       </c>
@@ -10036,7 +10140,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" ht="15" customHeight="1">
       <c r="A78" t="s">
         <v>97</v>
       </c>
@@ -10104,7 +10208,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" ht="15" customHeight="1">
       <c r="A79" t="s">
         <v>98</v>
       </c>
@@ -10172,7 +10276,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="80" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" ht="15" customHeight="1">
       <c r="A80" t="s">
         <v>99</v>
       </c>
@@ -10243,7 +10347,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" ht="15" customHeight="1">
       <c r="A81" t="s">
         <v>100</v>
       </c>
@@ -10311,7 +10415,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="15" customHeight="1">
       <c r="A82" t="s">
         <v>101</v>
       </c>
@@ -10382,7 +10486,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" ht="15" customHeight="1">
       <c r="A83" t="s">
         <v>102</v>
       </c>
@@ -10450,7 +10554,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="84" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" ht="15" customHeight="1">
       <c r="A84" t="s">
         <v>103</v>
       </c>
@@ -10521,7 +10625,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="85" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" ht="15" customHeight="1">
       <c r="A85" t="s">
         <v>104</v>
       </c>
@@ -10592,7 +10696,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" ht="15" customHeight="1">
       <c r="A86" t="s">
         <v>105</v>
       </c>
@@ -10663,7 +10767,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="87" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" ht="15" customHeight="1">
       <c r="A87" t="s">
         <v>106</v>
       </c>
@@ -10734,7 +10838,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" ht="15" customHeight="1">
       <c r="A88" t="s">
         <v>107</v>
       </c>
@@ -10802,7 +10906,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="15" customHeight="1">
       <c r="A89" t="s">
         <v>108</v>
       </c>
@@ -10873,7 +10977,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="90" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" ht="15" customHeight="1">
       <c r="A90" t="s">
         <v>109</v>
       </c>
@@ -10944,7 +11048,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="91" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" ht="15" customHeight="1">
       <c r="A91" t="s">
         <v>110</v>
       </c>
@@ -11012,7 +11116,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="92" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" ht="15" customHeight="1">
       <c r="A92" t="s">
         <v>111</v>
       </c>
@@ -11080,7 +11184,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="93" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" ht="15" customHeight="1">
       <c r="A93" t="s">
         <v>112</v>
       </c>
@@ -11151,7 +11255,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="15" customHeight="1">
       <c r="A94" t="s">
         <v>113</v>
       </c>
@@ -11219,7 +11323,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="95" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" ht="15" customHeight="1">
       <c r="A95" t="s">
         <v>114</v>
       </c>
@@ -11287,7 +11391,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="96" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" ht="15" customHeight="1">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -11355,7 +11459,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="97" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" ht="15" customHeight="1">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -11426,7 +11530,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="98" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" ht="15" customHeight="1">
       <c r="A98" t="s">
         <v>117</v>
       </c>
@@ -11494,7 +11598,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" ht="15" customHeight="1">
       <c r="A99" t="s">
         <v>118</v>
       </c>
@@ -11565,7 +11669,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" ht="15" customHeight="1">
       <c r="A100" t="s">
         <v>119</v>
       </c>
@@ -11636,7 +11740,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" ht="15" customHeight="1">
       <c r="A101" t="s">
         <v>120</v>
       </c>
@@ -11704,7 +11808,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" ht="15" customHeight="1">
       <c r="A102" t="s">
         <v>121</v>
       </c>
@@ -11772,7 +11876,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" ht="15" customHeight="1">
       <c r="A103" t="s">
         <v>122</v>
       </c>
@@ -11840,7 +11944,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" ht="15" customHeight="1">
       <c r="A104" t="s">
         <v>123</v>
       </c>
@@ -11908,7 +12012,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" ht="15" customHeight="1">
       <c r="A105" t="s">
         <v>124</v>
       </c>
@@ -11979,7 +12083,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" ht="15" customHeight="1">
       <c r="A106" t="s">
         <v>125</v>
       </c>
@@ -12047,7 +12151,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" ht="15" customHeight="1">
       <c r="A107" t="s">
         <v>126</v>
       </c>
@@ -12115,7 +12219,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" ht="15" customHeight="1">
       <c r="A108" t="s">
         <v>127</v>
       </c>
@@ -12183,7 +12287,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="109" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" ht="15" customHeight="1">
       <c r="A109" t="s">
         <v>128</v>
       </c>
@@ -12251,7 +12355,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" ht="15" customHeight="1">
       <c r="A110" t="s">
         <v>129</v>
       </c>
@@ -12322,7 +12426,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="111" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" ht="15" customHeight="1">
       <c r="A111" t="s">
         <v>130</v>
       </c>
@@ -12393,7 +12497,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="112" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" ht="15" customHeight="1">
       <c r="A112" t="s">
         <v>131</v>
       </c>
@@ -12464,7 +12568,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="113" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" ht="15" customHeight="1">
       <c r="A113" t="s">
         <v>132</v>
       </c>
@@ -12529,7 +12633,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="114" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" ht="15" customHeight="1">
       <c r="A114" t="s">
         <v>133</v>
       </c>
@@ -12597,7 +12701,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="115" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" ht="15" customHeight="1">
       <c r="A115" t="s">
         <v>134</v>
       </c>
@@ -12665,7 +12769,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="116" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" ht="15" customHeight="1">
       <c r="A116" t="s">
         <v>135</v>
       </c>
@@ -12733,7 +12837,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="117" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" ht="15" customHeight="1">
       <c r="A117" t="s">
         <v>136</v>
       </c>
@@ -12801,7 +12905,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="118" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:22" ht="15" customHeight="1">
       <c r="A118" t="s">
         <v>137</v>
       </c>
@@ -12860,7 +12964,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="119" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:22" ht="15" customHeight="1">
       <c r="A119" t="s">
         <v>138</v>
       </c>
@@ -12919,7 +13023,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="120" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" ht="15" customHeight="1">
       <c r="A120" t="s">
         <v>139</v>
       </c>
@@ -12987,7 +13091,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="121" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" ht="15" customHeight="1">
       <c r="A121" t="s">
         <v>140</v>
       </c>
@@ -13055,7 +13159,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="122" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" ht="15" customHeight="1">
       <c r="A122" t="s">
         <v>141</v>
       </c>
@@ -13123,7 +13227,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="123" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" ht="15" customHeight="1">
       <c r="A123" t="s">
         <v>142</v>
       </c>
@@ -13191,7 +13295,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="124" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" ht="15" customHeight="1">
       <c r="A124" t="s">
         <v>143</v>
       </c>
@@ -13259,7 +13363,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="125" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" ht="15" customHeight="1">
       <c r="A125" t="s">
         <v>144</v>
       </c>
@@ -13324,7 +13428,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="126" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" ht="15" customHeight="1">
       <c r="A126" t="s">
         <v>145</v>
       </c>
@@ -13392,7 +13496,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="127" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" ht="15" customHeight="1">
       <c r="A127" t="s">
         <v>146</v>
       </c>
@@ -13460,7 +13564,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="128" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" ht="15" customHeight="1">
       <c r="A128" t="s">
         <v>147</v>
       </c>
@@ -13531,7 +13635,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="129" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" ht="15" customHeight="1">
       <c r="A129" t="s">
         <v>148</v>
       </c>
@@ -13599,7 +13703,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="130" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:22" ht="15" customHeight="1">
       <c r="A130" t="s">
         <v>149</v>
       </c>
@@ -13661,7 +13765,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="131" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:23" ht="15" customHeight="1">
       <c r="A131" t="s">
         <v>150</v>
       </c>
@@ -13732,7 +13836,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="132" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:23" ht="15" customHeight="1">
       <c r="A132" t="s">
         <v>151</v>
       </c>
@@ -13803,7 +13907,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="133" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:23" ht="15" customHeight="1">
       <c r="A133" t="s">
         <v>152</v>
       </c>
@@ -13874,7 +13978,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="134" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:23" ht="15" customHeight="1">
       <c r="A134" t="s">
         <v>153</v>
       </c>
@@ -13945,7 +14049,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="135" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" ht="15" customHeight="1">
       <c r="A135" t="s">
         <v>154</v>
       </c>
@@ -13980,7 +14084,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="136" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" ht="15" customHeight="1">
       <c r="A136" t="s">
         <v>155</v>
       </c>
@@ -14015,7 +14119,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="137" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" ht="15" customHeight="1">
       <c r="A137" t="s">
         <v>156</v>
       </c>
@@ -14050,7 +14154,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="138" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" ht="15" customHeight="1">
       <c r="A138" t="s">
         <v>157</v>
       </c>
@@ -14085,7 +14189,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="139" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" ht="15" customHeight="1">
       <c r="A139" t="s">
         <v>158</v>
       </c>
@@ -14120,7 +14224,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="140" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" ht="15" customHeight="1">
       <c r="A140" t="s">
         <v>159</v>
       </c>
@@ -14155,7 +14259,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="141" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:17" ht="15" customHeight="1">
       <c r="A141" t="s">
         <v>160</v>
       </c>
@@ -14190,7 +14294,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="142" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" ht="15" customHeight="1">
       <c r="A142" t="s">
         <v>161</v>
       </c>
@@ -14225,7 +14329,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="143" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" ht="15" customHeight="1">
       <c r="A143" t="s">
         <v>162</v>
       </c>
@@ -14260,7 +14364,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="144" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" ht="15" customHeight="1">
       <c r="A144" t="s">
         <v>163</v>
       </c>
@@ -14295,7 +14399,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" ht="15" customHeight="1">
       <c r="A145" t="s">
         <v>164</v>
       </c>
@@ -14330,7 +14434,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" ht="15" customHeight="1">
       <c r="A146" t="s">
         <v>165</v>
       </c>
@@ -14365,7 +14469,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="147" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" ht="15" customHeight="1">
       <c r="A147" t="s">
         <v>166</v>
       </c>
@@ -14400,7 +14504,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" ht="15" customHeight="1">
       <c r="A148" t="s">
         <v>167</v>
       </c>
@@ -14435,7 +14539,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="149" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" ht="15" customHeight="1">
       <c r="A149" t="s">
         <v>168</v>
       </c>
@@ -14470,7 +14574,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" ht="15" customHeight="1">
       <c r="A150" t="s">
         <v>169</v>
       </c>
@@ -14507,592 +14611,592 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D150">
-    <cfRule type="containsText" dxfId="4" priority="23" operator="containsText" text="Editorial">
+    <cfRule type="containsText" priority="23" dxfId="4" operator="containsText" text="Editorial">
       <formula>NOT(ISERROR(SEARCH("Editorial",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L47 M2:O150">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="NOT">
+  <conditionalFormatting sqref="M2:O150 L47">
+    <cfRule type="containsText" priority="1" dxfId="3" operator="containsText" text="NOT">
       <formula>NOT(ISERROR(SEARCH("NOT",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L118:L119">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="NOT">
+    <cfRule type="containsText" priority="2" dxfId="3" operator="containsText" text="NOT">
       <formula>NOT(ISERROR(SEARCH("NOT",L118)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L130">
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="NOT">
+    <cfRule type="containsText" priority="4" dxfId="3" operator="containsText" text="NOT">
       <formula>NOT(ISERROR(SEARCH("NOT",L130)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:O150">
-    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Corpus">
+    <cfRule type="containsText" priority="6" dxfId="4" operator="containsText" text="Corpus">
       <formula>NOT(ISERROR(SEARCH("Corpus",L2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="J2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="L2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="R2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="I3" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="J3" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="R3" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="I4" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="J4" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="L4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="R4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="I5" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J5" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="L5" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="R5" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="I6" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="J6" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="R6" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="I7" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="J7" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="L7" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="R7" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="I8" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="J8" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L8" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="R8" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="I9" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="J9" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="R9" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="I10" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="J10" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="L10" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="R10" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="I11" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="J11" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="R11" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="I12" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="J12" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="L12" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="R12" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="I13" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="J13" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="L13" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="R13" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="I14" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="J14" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="R14" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="I15" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="J15" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="R15" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="I16" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="J16" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="R16" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="I17" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="J17" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="L17" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="R17" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="I18" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="J18" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="L18" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="R18" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="I19" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="J19" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="R19" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="I20" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="J20" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="L20" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="R20" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="I21" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="J21" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="L21" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="R21" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="I22" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="J22" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="L22" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="R22" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="I23" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="J23" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="L23" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="R23" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="I24" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="J24" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="L24" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="R24" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="I25" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="J25" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="L25" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="R25" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="I26" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="J26" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="R26" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="I27" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="J27" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="R27" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="I28" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="J28" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="L28" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="R28" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="I29" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="J29" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="L29" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="R29" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="I30" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="J30" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="R30" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="I31" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="J31" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="L31" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="R31" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="I32" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="J32" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="L32" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="R32" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="I33" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="J33" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="L33" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="R33" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="I34" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="J34" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="L34" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="R34" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="I35" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="J35" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="L35" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="R35" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="I36" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="J36" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="L36" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="R36" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="I37" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="J37" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="L37" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="R37" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="I38" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="J38" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="L38" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="R38" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="I39" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="J39" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="L39" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="R39" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="I40" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="J40" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
-    <hyperlink ref="L40" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="R40" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
-    <hyperlink ref="I41" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="J41" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="R41" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="I42" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="J42" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="L42" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="R42" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="I43" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="J43" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="L43" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="R43" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="I44" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="J44" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="L44" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="R44" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="I45" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="J45" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="R45" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="I46" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="J46" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="L46" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="R46" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="G47" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="G48" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="H48" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="I48" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="L48" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="R48" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="G49" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="H49" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="I49" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="L49" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="R49" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="G50" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="H50" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="I50" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="R50" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="G51" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="H51" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
-    <hyperlink ref="I51" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="L51" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="R51" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="G52" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
-    <hyperlink ref="H52" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="I52" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
-    <hyperlink ref="L52" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="R52" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
-    <hyperlink ref="G53" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
-    <hyperlink ref="H53" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
-    <hyperlink ref="I53" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
-    <hyperlink ref="R53" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="G54" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="H54" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="I54" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="R54" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="G55" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="H55" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="I55" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="L55" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
-    <hyperlink ref="R55" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="G56" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="H56" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="I56" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="L56" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="R56" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="G57" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="H57" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="I57" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="R57" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="G58" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="H58" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="I58" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="R58" r:id="rId218" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="G59" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="H59" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="I59" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="R59" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="G60" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="H60" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="I60" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="L60" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="R60" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="G61" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="H61" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="I61" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="R61" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="G62" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="H62" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="I62" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
-    <hyperlink ref="L62" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
-    <hyperlink ref="R62" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
-    <hyperlink ref="G63" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
-    <hyperlink ref="H63" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
-    <hyperlink ref="I63" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
-    <hyperlink ref="L63" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
-    <hyperlink ref="R63" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
-    <hyperlink ref="G64" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
-    <hyperlink ref="H64" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
-    <hyperlink ref="I64" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
-    <hyperlink ref="L64" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
-    <hyperlink ref="R64" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
-    <hyperlink ref="G65" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
-    <hyperlink ref="H65" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
-    <hyperlink ref="I65" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
-    <hyperlink ref="L65" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
-    <hyperlink ref="R65" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
-    <hyperlink ref="G66" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
-    <hyperlink ref="H66" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
-    <hyperlink ref="I66" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
-    <hyperlink ref="L66" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
-    <hyperlink ref="R66" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
-    <hyperlink ref="G67" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
-    <hyperlink ref="H67" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
-    <hyperlink ref="I67" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
-    <hyperlink ref="L67" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
-    <hyperlink ref="R67" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
-    <hyperlink ref="G68" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
-    <hyperlink ref="H68" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
-    <hyperlink ref="I68" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
-    <hyperlink ref="L68" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
-    <hyperlink ref="R68" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
-    <hyperlink ref="G69" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
-    <hyperlink ref="H69" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
-    <hyperlink ref="I69" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
-    <hyperlink ref="R69" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
-    <hyperlink ref="G70" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
-    <hyperlink ref="H70" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
-    <hyperlink ref="I70" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
-    <hyperlink ref="R70" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
-    <hyperlink ref="G71" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
-    <hyperlink ref="H71" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
-    <hyperlink ref="I71" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
-    <hyperlink ref="R71" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
-    <hyperlink ref="G72" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
-    <hyperlink ref="H72" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
-    <hyperlink ref="I72" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
-    <hyperlink ref="R72" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
-    <hyperlink ref="G73" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
-    <hyperlink ref="H73" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
-    <hyperlink ref="I73" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
-    <hyperlink ref="L73" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
-    <hyperlink ref="R73" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
-    <hyperlink ref="G74" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
-    <hyperlink ref="H74" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
-    <hyperlink ref="I74" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
-    <hyperlink ref="L74" r:id="rId291" xr:uid="{00000000-0004-0000-0000-000022010000}"/>
-    <hyperlink ref="R74" r:id="rId292" xr:uid="{00000000-0004-0000-0000-000023010000}"/>
-    <hyperlink ref="G75" r:id="rId293" xr:uid="{00000000-0004-0000-0000-000024010000}"/>
-    <hyperlink ref="H75" r:id="rId294" xr:uid="{00000000-0004-0000-0000-000025010000}"/>
-    <hyperlink ref="I75" r:id="rId295" xr:uid="{00000000-0004-0000-0000-000026010000}"/>
-    <hyperlink ref="L75" r:id="rId296" xr:uid="{00000000-0004-0000-0000-000027010000}"/>
-    <hyperlink ref="R75" r:id="rId297" xr:uid="{00000000-0004-0000-0000-000028010000}"/>
-    <hyperlink ref="G76" r:id="rId298" xr:uid="{00000000-0004-0000-0000-000029010000}"/>
-    <hyperlink ref="H76" r:id="rId299" xr:uid="{00000000-0004-0000-0000-00002A010000}"/>
-    <hyperlink ref="I76" r:id="rId300" xr:uid="{00000000-0004-0000-0000-00002B010000}"/>
-    <hyperlink ref="L76" r:id="rId301" xr:uid="{00000000-0004-0000-0000-00002C010000}"/>
-    <hyperlink ref="R76" r:id="rId302" xr:uid="{00000000-0004-0000-0000-00002D010000}"/>
-    <hyperlink ref="G77" r:id="rId303" xr:uid="{00000000-0004-0000-0000-00002E010000}"/>
-    <hyperlink ref="H77" r:id="rId304" xr:uid="{00000000-0004-0000-0000-00002F010000}"/>
-    <hyperlink ref="I77" r:id="rId305" xr:uid="{00000000-0004-0000-0000-000030010000}"/>
-    <hyperlink ref="L77" r:id="rId306" xr:uid="{00000000-0004-0000-0000-000031010000}"/>
-    <hyperlink ref="R77" r:id="rId307" xr:uid="{00000000-0004-0000-0000-000032010000}"/>
-    <hyperlink ref="G78" r:id="rId308" xr:uid="{00000000-0004-0000-0000-000033010000}"/>
-    <hyperlink ref="H78" r:id="rId309" xr:uid="{00000000-0004-0000-0000-000034010000}"/>
-    <hyperlink ref="I78" r:id="rId310" xr:uid="{00000000-0004-0000-0000-000035010000}"/>
-    <hyperlink ref="R78" r:id="rId311" xr:uid="{00000000-0004-0000-0000-000036010000}"/>
-    <hyperlink ref="G79" r:id="rId312" xr:uid="{00000000-0004-0000-0000-000037010000}"/>
-    <hyperlink ref="H79" r:id="rId313" xr:uid="{00000000-0004-0000-0000-000038010000}"/>
-    <hyperlink ref="I79" r:id="rId314" xr:uid="{00000000-0004-0000-0000-000039010000}"/>
-    <hyperlink ref="R79" r:id="rId315" xr:uid="{00000000-0004-0000-0000-00003A010000}"/>
-    <hyperlink ref="G80" r:id="rId316" xr:uid="{00000000-0004-0000-0000-00003B010000}"/>
-    <hyperlink ref="H80" r:id="rId317" xr:uid="{00000000-0004-0000-0000-00003C010000}"/>
-    <hyperlink ref="I80" r:id="rId318" xr:uid="{00000000-0004-0000-0000-00003D010000}"/>
-    <hyperlink ref="L80" r:id="rId319" xr:uid="{00000000-0004-0000-0000-00003E010000}"/>
-    <hyperlink ref="R80" r:id="rId320" xr:uid="{00000000-0004-0000-0000-00003F010000}"/>
-    <hyperlink ref="G81" r:id="rId321" xr:uid="{00000000-0004-0000-0000-000040010000}"/>
-    <hyperlink ref="H81" r:id="rId322" xr:uid="{00000000-0004-0000-0000-000041010000}"/>
-    <hyperlink ref="I81" r:id="rId323" xr:uid="{00000000-0004-0000-0000-000042010000}"/>
-    <hyperlink ref="L81" r:id="rId324" xr:uid="{00000000-0004-0000-0000-000043010000}"/>
-    <hyperlink ref="R81" r:id="rId325" xr:uid="{00000000-0004-0000-0000-000044010000}"/>
-    <hyperlink ref="G82" r:id="rId326" xr:uid="{00000000-0004-0000-0000-000045010000}"/>
-    <hyperlink ref="H82" r:id="rId327" xr:uid="{00000000-0004-0000-0000-000046010000}"/>
-    <hyperlink ref="I82" r:id="rId328" xr:uid="{00000000-0004-0000-0000-000047010000}"/>
-    <hyperlink ref="R82" r:id="rId329" xr:uid="{00000000-0004-0000-0000-000048010000}"/>
-    <hyperlink ref="G83" r:id="rId330" xr:uid="{00000000-0004-0000-0000-000049010000}"/>
-    <hyperlink ref="H83" r:id="rId331" xr:uid="{00000000-0004-0000-0000-00004A010000}"/>
-    <hyperlink ref="I83" r:id="rId332" xr:uid="{00000000-0004-0000-0000-00004B010000}"/>
-    <hyperlink ref="L83" r:id="rId333" xr:uid="{00000000-0004-0000-0000-00004C010000}"/>
-    <hyperlink ref="R83" r:id="rId334" xr:uid="{00000000-0004-0000-0000-00004D010000}"/>
-    <hyperlink ref="G84" r:id="rId335" xr:uid="{00000000-0004-0000-0000-00004E010000}"/>
-    <hyperlink ref="H84" r:id="rId336" xr:uid="{00000000-0004-0000-0000-00004F010000}"/>
-    <hyperlink ref="I84" r:id="rId337" xr:uid="{00000000-0004-0000-0000-000050010000}"/>
-    <hyperlink ref="R84" r:id="rId338" xr:uid="{00000000-0004-0000-0000-000051010000}"/>
-    <hyperlink ref="G85" r:id="rId339" xr:uid="{00000000-0004-0000-0000-000052010000}"/>
-    <hyperlink ref="H85" r:id="rId340" xr:uid="{00000000-0004-0000-0000-000053010000}"/>
-    <hyperlink ref="I85" r:id="rId341" xr:uid="{00000000-0004-0000-0000-000054010000}"/>
-    <hyperlink ref="R85" r:id="rId342" xr:uid="{00000000-0004-0000-0000-000055010000}"/>
-    <hyperlink ref="G86" r:id="rId343" xr:uid="{00000000-0004-0000-0000-000056010000}"/>
-    <hyperlink ref="H86" r:id="rId344" xr:uid="{00000000-0004-0000-0000-000057010000}"/>
-    <hyperlink ref="I86" r:id="rId345" xr:uid="{00000000-0004-0000-0000-000058010000}"/>
-    <hyperlink ref="R86" r:id="rId346" xr:uid="{00000000-0004-0000-0000-000059010000}"/>
-    <hyperlink ref="G87" r:id="rId347" xr:uid="{00000000-0004-0000-0000-00005A010000}"/>
-    <hyperlink ref="H87" r:id="rId348" xr:uid="{00000000-0004-0000-0000-00005B010000}"/>
-    <hyperlink ref="I87" r:id="rId349" xr:uid="{00000000-0004-0000-0000-00005C010000}"/>
-    <hyperlink ref="R87" r:id="rId350" xr:uid="{00000000-0004-0000-0000-00005D010000}"/>
-    <hyperlink ref="G88" r:id="rId351" xr:uid="{00000000-0004-0000-0000-00005E010000}"/>
-    <hyperlink ref="H88" r:id="rId352" xr:uid="{00000000-0004-0000-0000-00005F010000}"/>
-    <hyperlink ref="I88" r:id="rId353" xr:uid="{00000000-0004-0000-0000-000060010000}"/>
-    <hyperlink ref="R88" r:id="rId354" xr:uid="{00000000-0004-0000-0000-000061010000}"/>
-    <hyperlink ref="G89" r:id="rId355" xr:uid="{00000000-0004-0000-0000-000062010000}"/>
-    <hyperlink ref="H89" r:id="rId356" xr:uid="{00000000-0004-0000-0000-000063010000}"/>
-    <hyperlink ref="I89" r:id="rId357" xr:uid="{00000000-0004-0000-0000-000064010000}"/>
-    <hyperlink ref="L89" r:id="rId358" xr:uid="{00000000-0004-0000-0000-000065010000}"/>
-    <hyperlink ref="R89" r:id="rId359" xr:uid="{00000000-0004-0000-0000-000066010000}"/>
-    <hyperlink ref="G90" r:id="rId360" xr:uid="{00000000-0004-0000-0000-000067010000}"/>
-    <hyperlink ref="H90" r:id="rId361" xr:uid="{00000000-0004-0000-0000-000068010000}"/>
-    <hyperlink ref="I90" r:id="rId362" xr:uid="{00000000-0004-0000-0000-000069010000}"/>
-    <hyperlink ref="R90" r:id="rId363" xr:uid="{00000000-0004-0000-0000-00006A010000}"/>
-    <hyperlink ref="G91" r:id="rId364" xr:uid="{00000000-0004-0000-0000-00006B010000}"/>
-    <hyperlink ref="H91" r:id="rId365" xr:uid="{00000000-0004-0000-0000-00006C010000}"/>
-    <hyperlink ref="I91" r:id="rId366" xr:uid="{00000000-0004-0000-0000-00006D010000}"/>
-    <hyperlink ref="L91" r:id="rId367" xr:uid="{00000000-0004-0000-0000-00006E010000}"/>
-    <hyperlink ref="R91" r:id="rId368" xr:uid="{00000000-0004-0000-0000-00006F010000}"/>
-    <hyperlink ref="G92" r:id="rId369" xr:uid="{00000000-0004-0000-0000-000070010000}"/>
-    <hyperlink ref="H92" r:id="rId370" xr:uid="{00000000-0004-0000-0000-000071010000}"/>
-    <hyperlink ref="I92" r:id="rId371" xr:uid="{00000000-0004-0000-0000-000072010000}"/>
-    <hyperlink ref="L92" r:id="rId372" xr:uid="{00000000-0004-0000-0000-000073010000}"/>
-    <hyperlink ref="R92" r:id="rId373" xr:uid="{00000000-0004-0000-0000-000074010000}"/>
-    <hyperlink ref="G93" r:id="rId374" xr:uid="{00000000-0004-0000-0000-000075010000}"/>
-    <hyperlink ref="H93" r:id="rId375" xr:uid="{00000000-0004-0000-0000-000076010000}"/>
-    <hyperlink ref="I93" r:id="rId376" xr:uid="{00000000-0004-0000-0000-000077010000}"/>
-    <hyperlink ref="R93" r:id="rId377" xr:uid="{00000000-0004-0000-0000-000078010000}"/>
-    <hyperlink ref="G94" r:id="rId378" xr:uid="{00000000-0004-0000-0000-000079010000}"/>
-    <hyperlink ref="H94" r:id="rId379" xr:uid="{00000000-0004-0000-0000-00007A010000}"/>
-    <hyperlink ref="I94" r:id="rId380" xr:uid="{00000000-0004-0000-0000-00007B010000}"/>
-    <hyperlink ref="L94" r:id="rId381" xr:uid="{00000000-0004-0000-0000-00007C010000}"/>
-    <hyperlink ref="R94" r:id="rId382" xr:uid="{00000000-0004-0000-0000-00007D010000}"/>
-    <hyperlink ref="G95" r:id="rId383" xr:uid="{00000000-0004-0000-0000-00007E010000}"/>
-    <hyperlink ref="H95" r:id="rId384" xr:uid="{00000000-0004-0000-0000-00007F010000}"/>
-    <hyperlink ref="I95" r:id="rId385" xr:uid="{00000000-0004-0000-0000-000080010000}"/>
-    <hyperlink ref="L95" r:id="rId386" xr:uid="{00000000-0004-0000-0000-000081010000}"/>
-    <hyperlink ref="R95" r:id="rId387" xr:uid="{00000000-0004-0000-0000-000082010000}"/>
-    <hyperlink ref="G96" r:id="rId388" xr:uid="{00000000-0004-0000-0000-000083010000}"/>
-    <hyperlink ref="H96" r:id="rId389" xr:uid="{00000000-0004-0000-0000-000084010000}"/>
-    <hyperlink ref="I96" r:id="rId390" xr:uid="{00000000-0004-0000-0000-000085010000}"/>
-    <hyperlink ref="L96" r:id="rId391" xr:uid="{00000000-0004-0000-0000-000086010000}"/>
-    <hyperlink ref="R96" r:id="rId392" xr:uid="{00000000-0004-0000-0000-000087010000}"/>
-    <hyperlink ref="G97" r:id="rId393" xr:uid="{00000000-0004-0000-0000-000088010000}"/>
-    <hyperlink ref="H97" r:id="rId394" xr:uid="{00000000-0004-0000-0000-000089010000}"/>
-    <hyperlink ref="I97" r:id="rId395" xr:uid="{00000000-0004-0000-0000-00008A010000}"/>
-    <hyperlink ref="L97" r:id="rId396" xr:uid="{00000000-0004-0000-0000-00008B010000}"/>
-    <hyperlink ref="R97" r:id="rId397" xr:uid="{00000000-0004-0000-0000-00008C010000}"/>
-    <hyperlink ref="G98" r:id="rId398" xr:uid="{00000000-0004-0000-0000-00008D010000}"/>
-    <hyperlink ref="H98" r:id="rId399" xr:uid="{00000000-0004-0000-0000-00008E010000}"/>
-    <hyperlink ref="I98" r:id="rId400" xr:uid="{00000000-0004-0000-0000-00008F010000}"/>
-    <hyperlink ref="R98" r:id="rId401" xr:uid="{00000000-0004-0000-0000-000090010000}"/>
-    <hyperlink ref="G99" r:id="rId402" xr:uid="{00000000-0004-0000-0000-000091010000}"/>
-    <hyperlink ref="H99" r:id="rId403" xr:uid="{00000000-0004-0000-0000-000092010000}"/>
-    <hyperlink ref="I99" r:id="rId404" xr:uid="{00000000-0004-0000-0000-000093010000}"/>
-    <hyperlink ref="L99" r:id="rId405" xr:uid="{00000000-0004-0000-0000-000094010000}"/>
-    <hyperlink ref="R99" r:id="rId406" xr:uid="{00000000-0004-0000-0000-000095010000}"/>
-    <hyperlink ref="G100" r:id="rId407" xr:uid="{00000000-0004-0000-0000-000096010000}"/>
-    <hyperlink ref="H100" r:id="rId408" xr:uid="{00000000-0004-0000-0000-000097010000}"/>
-    <hyperlink ref="I100" r:id="rId409" xr:uid="{00000000-0004-0000-0000-000098010000}"/>
-    <hyperlink ref="R100" r:id="rId410" xr:uid="{00000000-0004-0000-0000-000099010000}"/>
-    <hyperlink ref="G101" r:id="rId411" xr:uid="{00000000-0004-0000-0000-00009A010000}"/>
-    <hyperlink ref="H101" r:id="rId412" xr:uid="{00000000-0004-0000-0000-00009B010000}"/>
-    <hyperlink ref="I101" r:id="rId413" xr:uid="{00000000-0004-0000-0000-00009C010000}"/>
-    <hyperlink ref="L101" r:id="rId414" xr:uid="{00000000-0004-0000-0000-00009D010000}"/>
-    <hyperlink ref="R101" r:id="rId415" xr:uid="{00000000-0004-0000-0000-00009E010000}"/>
-    <hyperlink ref="G102" r:id="rId416" xr:uid="{00000000-0004-0000-0000-00009F010000}"/>
-    <hyperlink ref="H102" r:id="rId417" xr:uid="{00000000-0004-0000-0000-0000A0010000}"/>
-    <hyperlink ref="I102" r:id="rId418" xr:uid="{00000000-0004-0000-0000-0000A1010000}"/>
-    <hyperlink ref="R102" r:id="rId419" xr:uid="{00000000-0004-0000-0000-0000A2010000}"/>
-    <hyperlink ref="G103" r:id="rId420" xr:uid="{00000000-0004-0000-0000-0000A3010000}"/>
-    <hyperlink ref="H103" r:id="rId421" xr:uid="{00000000-0004-0000-0000-0000A4010000}"/>
-    <hyperlink ref="I103" r:id="rId422" xr:uid="{00000000-0004-0000-0000-0000A5010000}"/>
-    <hyperlink ref="L103" r:id="rId423" xr:uid="{00000000-0004-0000-0000-0000A6010000}"/>
-    <hyperlink ref="R103" r:id="rId424" xr:uid="{00000000-0004-0000-0000-0000A7010000}"/>
-    <hyperlink ref="G104" r:id="rId425" xr:uid="{00000000-0004-0000-0000-0000A8010000}"/>
-    <hyperlink ref="H104" r:id="rId426" xr:uid="{00000000-0004-0000-0000-0000A9010000}"/>
-    <hyperlink ref="I104" r:id="rId427" xr:uid="{00000000-0004-0000-0000-0000AA010000}"/>
-    <hyperlink ref="L104" r:id="rId428" xr:uid="{00000000-0004-0000-0000-0000AB010000}"/>
-    <hyperlink ref="R104" r:id="rId429" xr:uid="{00000000-0004-0000-0000-0000AC010000}"/>
-    <hyperlink ref="G105" r:id="rId430" xr:uid="{00000000-0004-0000-0000-0000AD010000}"/>
-    <hyperlink ref="I105" r:id="rId431" xr:uid="{00000000-0004-0000-0000-0000AE010000}"/>
-    <hyperlink ref="R105" r:id="rId432" xr:uid="{00000000-0004-0000-0000-0000AF010000}"/>
-    <hyperlink ref="G106" r:id="rId433" xr:uid="{00000000-0004-0000-0000-0000B0010000}"/>
-    <hyperlink ref="H106" r:id="rId434" xr:uid="{00000000-0004-0000-0000-0000B1010000}"/>
-    <hyperlink ref="I106" r:id="rId435" xr:uid="{00000000-0004-0000-0000-0000B2010000}"/>
-    <hyperlink ref="R106" r:id="rId436" xr:uid="{00000000-0004-0000-0000-0000B3010000}"/>
-    <hyperlink ref="G107" r:id="rId437" xr:uid="{00000000-0004-0000-0000-0000B4010000}"/>
-    <hyperlink ref="H107" r:id="rId438" xr:uid="{00000000-0004-0000-0000-0000B5010000}"/>
-    <hyperlink ref="I107" r:id="rId439" xr:uid="{00000000-0004-0000-0000-0000B6010000}"/>
-    <hyperlink ref="R107" r:id="rId440" xr:uid="{00000000-0004-0000-0000-0000B7010000}"/>
-    <hyperlink ref="G108" r:id="rId441" xr:uid="{00000000-0004-0000-0000-0000B8010000}"/>
-    <hyperlink ref="H108" r:id="rId442" xr:uid="{00000000-0004-0000-0000-0000B9010000}"/>
-    <hyperlink ref="I108" r:id="rId443" xr:uid="{00000000-0004-0000-0000-0000BA010000}"/>
-    <hyperlink ref="L108" r:id="rId444" xr:uid="{00000000-0004-0000-0000-0000BB010000}"/>
-    <hyperlink ref="R108" r:id="rId445" xr:uid="{00000000-0004-0000-0000-0000BC010000}"/>
-    <hyperlink ref="G109" r:id="rId446" xr:uid="{00000000-0004-0000-0000-0000BD010000}"/>
-    <hyperlink ref="H109" r:id="rId447" xr:uid="{00000000-0004-0000-0000-0000BE010000}"/>
-    <hyperlink ref="I109" r:id="rId448" xr:uid="{00000000-0004-0000-0000-0000BF010000}"/>
-    <hyperlink ref="R109" r:id="rId449" xr:uid="{00000000-0004-0000-0000-0000C0010000}"/>
-    <hyperlink ref="G110" r:id="rId450" xr:uid="{00000000-0004-0000-0000-0000C1010000}"/>
-    <hyperlink ref="H110" r:id="rId451" xr:uid="{00000000-0004-0000-0000-0000C2010000}"/>
-    <hyperlink ref="I110" r:id="rId452" xr:uid="{00000000-0004-0000-0000-0000C3010000}"/>
-    <hyperlink ref="L110" r:id="rId453" xr:uid="{00000000-0004-0000-0000-0000C4010000}"/>
-    <hyperlink ref="R110" r:id="rId454" xr:uid="{00000000-0004-0000-0000-0000C5010000}"/>
-    <hyperlink ref="G111" r:id="rId455" xr:uid="{00000000-0004-0000-0000-0000C6010000}"/>
-    <hyperlink ref="H111" r:id="rId456" xr:uid="{00000000-0004-0000-0000-0000C7010000}"/>
-    <hyperlink ref="I111" r:id="rId457" xr:uid="{00000000-0004-0000-0000-0000C8010000}"/>
-    <hyperlink ref="L111" r:id="rId458" xr:uid="{00000000-0004-0000-0000-0000C9010000}"/>
-    <hyperlink ref="R111" r:id="rId459" xr:uid="{00000000-0004-0000-0000-0000CA010000}"/>
-    <hyperlink ref="G112" r:id="rId460" xr:uid="{00000000-0004-0000-0000-0000CB010000}"/>
-    <hyperlink ref="H112" r:id="rId461" xr:uid="{00000000-0004-0000-0000-0000CC010000}"/>
-    <hyperlink ref="I112" r:id="rId462" xr:uid="{00000000-0004-0000-0000-0000CD010000}"/>
-    <hyperlink ref="L112" r:id="rId463" xr:uid="{00000000-0004-0000-0000-0000CE010000}"/>
-    <hyperlink ref="R112" r:id="rId464" xr:uid="{00000000-0004-0000-0000-0000CF010000}"/>
-    <hyperlink ref="G113" r:id="rId465" xr:uid="{00000000-0004-0000-0000-0000D0010000}"/>
-    <hyperlink ref="H113" r:id="rId466" xr:uid="{00000000-0004-0000-0000-0000D1010000}"/>
-    <hyperlink ref="I113" r:id="rId467" xr:uid="{00000000-0004-0000-0000-0000D2010000}"/>
-    <hyperlink ref="G114" r:id="rId468" xr:uid="{00000000-0004-0000-0000-0000D3010000}"/>
-    <hyperlink ref="H114" r:id="rId469" xr:uid="{00000000-0004-0000-0000-0000D4010000}"/>
-    <hyperlink ref="I114" r:id="rId470" xr:uid="{00000000-0004-0000-0000-0000D5010000}"/>
-    <hyperlink ref="L114" r:id="rId471" xr:uid="{00000000-0004-0000-0000-0000D6010000}"/>
-    <hyperlink ref="R114" r:id="rId472" xr:uid="{00000000-0004-0000-0000-0000D7010000}"/>
-    <hyperlink ref="G115" r:id="rId473" xr:uid="{00000000-0004-0000-0000-0000D8010000}"/>
-    <hyperlink ref="H115" r:id="rId474" xr:uid="{00000000-0004-0000-0000-0000D9010000}"/>
-    <hyperlink ref="I115" r:id="rId475" xr:uid="{00000000-0004-0000-0000-0000DA010000}"/>
-    <hyperlink ref="L115" r:id="rId476" xr:uid="{00000000-0004-0000-0000-0000DB010000}"/>
-    <hyperlink ref="R115" r:id="rId477" xr:uid="{00000000-0004-0000-0000-0000DC010000}"/>
-    <hyperlink ref="G116" r:id="rId478" xr:uid="{00000000-0004-0000-0000-0000DD010000}"/>
-    <hyperlink ref="H116" r:id="rId479" xr:uid="{00000000-0004-0000-0000-0000DE010000}"/>
-    <hyperlink ref="I116" r:id="rId480" xr:uid="{00000000-0004-0000-0000-0000DF010000}"/>
-    <hyperlink ref="L116" r:id="rId481" xr:uid="{00000000-0004-0000-0000-0000E0010000}"/>
-    <hyperlink ref="R116" r:id="rId482" xr:uid="{00000000-0004-0000-0000-0000E1010000}"/>
-    <hyperlink ref="G117" r:id="rId483" xr:uid="{00000000-0004-0000-0000-0000E2010000}"/>
-    <hyperlink ref="H117" r:id="rId484" xr:uid="{00000000-0004-0000-0000-0000E3010000}"/>
-    <hyperlink ref="I117" r:id="rId485" xr:uid="{00000000-0004-0000-0000-0000E4010000}"/>
-    <hyperlink ref="L117" r:id="rId486" xr:uid="{00000000-0004-0000-0000-0000E5010000}"/>
-    <hyperlink ref="R117" r:id="rId487" xr:uid="{00000000-0004-0000-0000-0000E6010000}"/>
-    <hyperlink ref="G118" r:id="rId488" xr:uid="{00000000-0004-0000-0000-0000E7010000}"/>
-    <hyperlink ref="G119" r:id="rId489" xr:uid="{00000000-0004-0000-0000-0000E8010000}"/>
-    <hyperlink ref="G120" r:id="rId490" xr:uid="{00000000-0004-0000-0000-0000E9010000}"/>
-    <hyperlink ref="H120" r:id="rId491" xr:uid="{00000000-0004-0000-0000-0000EA010000}"/>
-    <hyperlink ref="I120" r:id="rId492" xr:uid="{00000000-0004-0000-0000-0000EB010000}"/>
-    <hyperlink ref="L120" r:id="rId493" xr:uid="{00000000-0004-0000-0000-0000EC010000}"/>
-    <hyperlink ref="R120" r:id="rId494" xr:uid="{00000000-0004-0000-0000-0000ED010000}"/>
-    <hyperlink ref="G121" r:id="rId495" xr:uid="{00000000-0004-0000-0000-0000EE010000}"/>
-    <hyperlink ref="H121" r:id="rId496" xr:uid="{00000000-0004-0000-0000-0000EF010000}"/>
-    <hyperlink ref="I121" r:id="rId497" xr:uid="{00000000-0004-0000-0000-0000F0010000}"/>
-    <hyperlink ref="L121" r:id="rId498" xr:uid="{00000000-0004-0000-0000-0000F1010000}"/>
-    <hyperlink ref="R121" r:id="rId499" xr:uid="{00000000-0004-0000-0000-0000F2010000}"/>
-    <hyperlink ref="G122" r:id="rId500" xr:uid="{00000000-0004-0000-0000-0000F3010000}"/>
-    <hyperlink ref="H122" r:id="rId501" xr:uid="{00000000-0004-0000-0000-0000F4010000}"/>
-    <hyperlink ref="I122" r:id="rId502" xr:uid="{00000000-0004-0000-0000-0000F5010000}"/>
-    <hyperlink ref="L122" r:id="rId503" xr:uid="{00000000-0004-0000-0000-0000F6010000}"/>
-    <hyperlink ref="R122" r:id="rId504" xr:uid="{00000000-0004-0000-0000-0000F7010000}"/>
-    <hyperlink ref="G123" r:id="rId505" xr:uid="{00000000-0004-0000-0000-0000F8010000}"/>
-    <hyperlink ref="H123" r:id="rId506" xr:uid="{00000000-0004-0000-0000-0000F9010000}"/>
-    <hyperlink ref="I123" r:id="rId507" xr:uid="{00000000-0004-0000-0000-0000FA010000}"/>
-    <hyperlink ref="L123" r:id="rId508" xr:uid="{00000000-0004-0000-0000-0000FB010000}"/>
-    <hyperlink ref="R123" r:id="rId509" xr:uid="{00000000-0004-0000-0000-0000FC010000}"/>
-    <hyperlink ref="G124" r:id="rId510" xr:uid="{00000000-0004-0000-0000-0000FD010000}"/>
-    <hyperlink ref="H124" r:id="rId511" xr:uid="{00000000-0004-0000-0000-0000FE010000}"/>
-    <hyperlink ref="I124" r:id="rId512" xr:uid="{00000000-0004-0000-0000-0000FF010000}"/>
-    <hyperlink ref="L124" r:id="rId513" xr:uid="{00000000-0004-0000-0000-000000020000}"/>
-    <hyperlink ref="R124" r:id="rId514" xr:uid="{00000000-0004-0000-0000-000001020000}"/>
-    <hyperlink ref="G125" r:id="rId515" xr:uid="{00000000-0004-0000-0000-000002020000}"/>
-    <hyperlink ref="H125" r:id="rId516" xr:uid="{00000000-0004-0000-0000-000003020000}"/>
-    <hyperlink ref="I125" r:id="rId517" xr:uid="{00000000-0004-0000-0000-000004020000}"/>
-    <hyperlink ref="L125" r:id="rId518" xr:uid="{00000000-0004-0000-0000-000005020000}"/>
-    <hyperlink ref="G126" r:id="rId519" xr:uid="{00000000-0004-0000-0000-000006020000}"/>
-    <hyperlink ref="H126" r:id="rId520" xr:uid="{00000000-0004-0000-0000-000007020000}"/>
-    <hyperlink ref="I126" r:id="rId521" xr:uid="{00000000-0004-0000-0000-000008020000}"/>
-    <hyperlink ref="L126" r:id="rId522" xr:uid="{00000000-0004-0000-0000-000009020000}"/>
-    <hyperlink ref="R126" r:id="rId523" xr:uid="{00000000-0004-0000-0000-00000A020000}"/>
-    <hyperlink ref="G127" r:id="rId524" xr:uid="{00000000-0004-0000-0000-00000B020000}"/>
-    <hyperlink ref="H127" r:id="rId525" xr:uid="{00000000-0004-0000-0000-00000C020000}"/>
-    <hyperlink ref="I127" r:id="rId526" xr:uid="{00000000-0004-0000-0000-00000D020000}"/>
-    <hyperlink ref="L127" r:id="rId527" xr:uid="{00000000-0004-0000-0000-00000E020000}"/>
-    <hyperlink ref="R127" r:id="rId528" xr:uid="{00000000-0004-0000-0000-00000F020000}"/>
-    <hyperlink ref="G128" r:id="rId529" xr:uid="{00000000-0004-0000-0000-000010020000}"/>
-    <hyperlink ref="H128" r:id="rId530" xr:uid="{00000000-0004-0000-0000-000011020000}"/>
-    <hyperlink ref="I128" r:id="rId531" xr:uid="{00000000-0004-0000-0000-000012020000}"/>
-    <hyperlink ref="L128" r:id="rId532" xr:uid="{00000000-0004-0000-0000-000013020000}"/>
-    <hyperlink ref="R128" r:id="rId533" xr:uid="{00000000-0004-0000-0000-000014020000}"/>
-    <hyperlink ref="G129" r:id="rId534" xr:uid="{00000000-0004-0000-0000-000015020000}"/>
-    <hyperlink ref="H129" r:id="rId535" xr:uid="{00000000-0004-0000-0000-000016020000}"/>
-    <hyperlink ref="I129" r:id="rId536" xr:uid="{00000000-0004-0000-0000-000017020000}"/>
-    <hyperlink ref="L129" r:id="rId537" xr:uid="{00000000-0004-0000-0000-000018020000}"/>
-    <hyperlink ref="R129" r:id="rId538" xr:uid="{00000000-0004-0000-0000-000019020000}"/>
-    <hyperlink ref="G130" r:id="rId539" xr:uid="{00000000-0004-0000-0000-00001A020000}"/>
-    <hyperlink ref="R130" r:id="rId540" xr:uid="{00000000-0004-0000-0000-00001B020000}"/>
-    <hyperlink ref="G131" r:id="rId541" xr:uid="{00000000-0004-0000-0000-00001C020000}"/>
-    <hyperlink ref="H131" r:id="rId542" xr:uid="{00000000-0004-0000-0000-00001D020000}"/>
-    <hyperlink ref="I131" r:id="rId543" xr:uid="{00000000-0004-0000-0000-00001E020000}"/>
-    <hyperlink ref="L131" r:id="rId544" xr:uid="{00000000-0004-0000-0000-00001F020000}"/>
-    <hyperlink ref="R131" r:id="rId545" xr:uid="{00000000-0004-0000-0000-000020020000}"/>
-    <hyperlink ref="G132" r:id="rId546" xr:uid="{00000000-0004-0000-0000-000021020000}"/>
-    <hyperlink ref="H132" r:id="rId547" xr:uid="{00000000-0004-0000-0000-000022020000}"/>
-    <hyperlink ref="I132" r:id="rId548" xr:uid="{00000000-0004-0000-0000-000023020000}"/>
-    <hyperlink ref="R132" r:id="rId549" xr:uid="{00000000-0004-0000-0000-000024020000}"/>
-    <hyperlink ref="G133" r:id="rId550" xr:uid="{00000000-0004-0000-0000-000025020000}"/>
-    <hyperlink ref="H133" r:id="rId551" xr:uid="{00000000-0004-0000-0000-000026020000}"/>
-    <hyperlink ref="I133" r:id="rId552" xr:uid="{00000000-0004-0000-0000-000027020000}"/>
-    <hyperlink ref="L133" r:id="rId553" xr:uid="{00000000-0004-0000-0000-000028020000}"/>
-    <hyperlink ref="R133" r:id="rId554" xr:uid="{00000000-0004-0000-0000-000029020000}"/>
-    <hyperlink ref="G134" r:id="rId555" xr:uid="{00000000-0004-0000-0000-00002A020000}"/>
-    <hyperlink ref="H134" r:id="rId556" xr:uid="{00000000-0004-0000-0000-00002B020000}"/>
-    <hyperlink ref="I134" r:id="rId557" xr:uid="{00000000-0004-0000-0000-00002C020000}"/>
-    <hyperlink ref="L134" r:id="rId558" xr:uid="{00000000-0004-0000-0000-00002D020000}"/>
-    <hyperlink ref="R134" r:id="rId559" xr:uid="{00000000-0004-0000-0000-00002E020000}"/>
+    <hyperlink ref="I2" r:id="rId1" display="https://proceedings.mlr.press/v162/han22c.html"/>
+    <hyperlink ref="J2" r:id="rId2" display="https://www.doi.org/10.5281/zenodo.8173650"/>
+    <hyperlink ref="L2" r:id="rId3" display="https://doi.org/10.48550/arXiv.2202.07179"/>
+    <hyperlink ref="R2" r:id="rId4" display="https://openreview.net/forum?id=XxUIomN-ndH"/>
+    <hyperlink ref="I3" r:id="rId5" display="https://openaccess.thecvf.com/content/CVPR2022/papers/Zhang_Exact_Feature_Distribution_Matching_for_Arbitrary_Style_Transfer_and_Domain_CVPR_2022_paper.pdf"/>
+    <hyperlink ref="J3" r:id="rId6" display="https://www.doi.org/10.5281/zenodo.8173652"/>
+    <hyperlink ref="R3" r:id="rId7" display="https://openreview.net/forum?id=a5_hbZf0NB&amp;noteId=Rsj9NvSj2Ft"/>
+    <hyperlink ref="I4" r:id="rId8" display="https://arxiv.org/pdf/2202.05826.pdf"/>
+    <hyperlink ref="J4" r:id="rId9" display="https://www.doi.org/10.5281/zenodo.8173654"/>
+    <hyperlink ref="L4" r:id="rId10" display="https://doi.org/10.48550/arXiv.2202.05826"/>
+    <hyperlink ref="R4" r:id="rId11" display="https://openreview.net/forum?id=WaZB4pUVTi"/>
+    <hyperlink ref="I5" r:id="rId12" display="https://proceedings.mlr.press/v162/crabbe22a.html"/>
+    <hyperlink ref="J5" r:id="rId13" display="https://www.doi.org/10.5281/zenodo.8173656"/>
+    <hyperlink ref="L5" r:id="rId14" display="https://doi.org/10.48550/arXiv.2203.01928"/>
+    <hyperlink ref="R5" r:id="rId15" display="https://openreview.net/forum?id=bBVZ3pY4z8p"/>
+    <hyperlink ref="I6" r:id="rId16" display="https://aclanthology.org/2021.acl-long.281/"/>
+    <hyperlink ref="J6" r:id="rId17" display="https://www.doi.org/10.5281/zenodo.8173658"/>
+    <hyperlink ref="R6" r:id="rId18" display="https://openreview.net/forum?id=Od5dD58libt"/>
+    <hyperlink ref="I7" r:id="rId19" display="https://proceedings.neurips.cc/paper/2021/hash/628f16b29939d1b060af49f66ae0f7f8-Abstract.html"/>
+    <hyperlink ref="J7" r:id="rId20" display="https://www.doi.org/10.5281/zenodo.8173662"/>
+    <hyperlink ref="L7" r:id="rId21" display="https://doi.org/10.48550/arXiv.2011.02803"/>
+    <hyperlink ref="R7" r:id="rId22" display="https://openreview.net/forum?id=gb71irTNN7"/>
+    <hyperlink ref="I8" r:id="rId23" display="https://neurips.cc/Conferences/2022/ScheduleMultitrack?event=53784"/>
+    <hyperlink ref="J8" r:id="rId24" display="https://www.doi.org/10.5281/zenodo.8173664"/>
+    <hyperlink ref="L8" r:id="rId25" display="https://doi.org/10.48550/arXiv.2206.02092"/>
+    <hyperlink ref="R8" r:id="rId26" display="https://openreview.net/forum?id=NE_x1dpz-Q"/>
+    <hyperlink ref="I9" r:id="rId27" display="https://openaccess.thecvf.com/content/CVPR2022/papers/Lim_Hypergraph-Induced_Semantic_Tuplet_Loss_for_Deep_Metric_Learning_CVPR_2022_paper.pdf"/>
+    <hyperlink ref="J9" r:id="rId28" display="https://www.doi.org/10.5281/zenodo.8173666"/>
+    <hyperlink ref="R9" r:id="rId29" display="https://openreview.net/forum?id=JJQbk2hIQ5"/>
+    <hyperlink ref="I10" r:id="rId30" display="https://openreview.net/forum?id=ao30zaT3YL"/>
+    <hyperlink ref="J10" r:id="rId31" display="https://www.doi.org/10.5281/zenodo.8173668"/>
+    <hyperlink ref="L10" r:id="rId32" display="https://doi.org/10.48550/arXiv.2205.10279"/>
+    <hyperlink ref="R10" r:id="rId33" display="https://openreview.net/forum?id=JpaQ8GFOVu"/>
+    <hyperlink ref="I11" r:id="rId34" display="https://doi.org/10.1007/978-3-031-19775-8_26"/>
+    <hyperlink ref="J11" r:id="rId35" display="https://www.doi.org/10.5281/zenodo.8173672"/>
+    <hyperlink ref="R11" r:id="rId36" display="https://openreview.net/forum?id=MK4IQJdLLeo"/>
+    <hyperlink ref="I12" r:id="rId37" display="https://proceedings.mlr.press/v162/crabbe22a/crabbe22a.pdf"/>
+    <hyperlink ref="J12" r:id="rId38" display="https://www.doi.org/10.5281/zenodo.8173674"/>
+    <hyperlink ref="L12" r:id="rId39" display="https://doi.org/10.48550/arXiv.2203.01928"/>
+    <hyperlink ref="R12" r:id="rId40" display="https://openreview.net/forum?id=qP34dvJpHd"/>
+    <hyperlink ref="I13" r:id="rId41" display="https://arxiv.org/abs/1911.12199"/>
+    <hyperlink ref="J13" r:id="rId42" display="https://www.doi.org/10.5281/zenodo.8173678"/>
+    <hyperlink ref="L13" r:id="rId43" display="https://doi.org/10.48550/arXiv.1911.12199"/>
+    <hyperlink ref="R13" r:id="rId44" display="https://openreview.net/forum?id=n1q-iz83S5&amp;noteId=60kzDmcWau"/>
+    <hyperlink ref="I14" r:id="rId45" display="https://iclr.cc/virtual/2022/poster/6666"/>
+    <hyperlink ref="J14" r:id="rId46" display="https://www.doi.org/10.5281/zenodo.8173680"/>
+    <hyperlink ref="R14" r:id="rId47" display="https://openreview.net/forum?id=xEfg6h1GFmW&amp;noteId=C0AfhPXAYB"/>
+    <hyperlink ref="I15" r:id="rId48" display="https://aclanthology.org/2022.naacl-main.418/"/>
+    <hyperlink ref="J15" r:id="rId49" display="https://www.doi.org/10.5281/zenodo.8173682"/>
+    <hyperlink ref="R15" r:id="rId50" display="https://openreview.net/forum?id=3jaZ5tKRyiT&amp;noteId=AHjI9Jw6frY"/>
+    <hyperlink ref="I16" r:id="rId51" display="https://openreview.net/pdf?id=nRj0NcmSuxb"/>
+    <hyperlink ref="J16" r:id="rId52" display="https://www.doi.org/10.5281/zenodo.8173686"/>
+    <hyperlink ref="R16" r:id="rId53" display="https://openreview.net/forum?id=uVHUy7CWCL"/>
+    <hyperlink ref="I17" r:id="rId54" display="https://proceedings.mlr.press/v162/crabbe22a/crabbe22a.pdf"/>
+    <hyperlink ref="J17" r:id="rId55" display="https://www.doi.org/10.5281/zenodo.8173688"/>
+    <hyperlink ref="L17" r:id="rId56" display="https://doi.org/10.48550/arXiv.2203.01928"/>
+    <hyperlink ref="R17" r:id="rId57" display="https://openreview.net/forum?id=sF_vYZSxSV"/>
+    <hyperlink ref="I18" r:id="rId58" display="https://proceedings.neurips.cc/paper/2021/file/043ab21fc5a1607b381ac3896176dac6-Paper.pdf"/>
+    <hyperlink ref="J18" r:id="rId59" display="https://www.doi.org/10.5281/zenodo.8173692"/>
+    <hyperlink ref="L18" r:id="rId60" display="https://doi.org/10.48550/arXiv.2106.12915"/>
+    <hyperlink ref="R18" r:id="rId61" display="https://openreview.net/forum?id=YAWQTQZVoA"/>
+    <hyperlink ref="I19" r:id="rId62" display="https://openreview.net/forum?id=wbPObLm6ueA"/>
+    <hyperlink ref="J19" r:id="rId63" display="https://www.doi.org/10.5281/zenodo.8206607"/>
+    <hyperlink ref="R19" r:id="rId64" display="https://openreview.net/forum?id=MMuv-v99Hy"/>
+    <hyperlink ref="I20" r:id="rId65" display="https://icml.cc/virtual/2022/poster/16829"/>
+    <hyperlink ref="J20" r:id="rId66" display="https://www.doi.org/10.5281/zenodo.8173696"/>
+    <hyperlink ref="L20" r:id="rId67" display="https://doi.org/10.48550/arXiv.2202.00858"/>
+    <hyperlink ref="R20" r:id="rId68" display="https://openreview.net/forum?id=NgPQSqpz-Y"/>
+    <hyperlink ref="I21" r:id="rId69" display="https://arxiv.org/abs/2205.00048"/>
+    <hyperlink ref="J21" r:id="rId70" display="https://www.doi.org/10.5281/zenodo.8173698"/>
+    <hyperlink ref="L21" r:id="rId71" display="https://doi.org/10.48550/arXiv.2205.00048"/>
+    <hyperlink ref="R21" r:id="rId72" display="https://openreview.net/forum?id=A0Sjs3IJWb-"/>
+    <hyperlink ref="I22" r:id="rId73" display="https://arxiv.org/abs/2203.15395"/>
+    <hyperlink ref="J22" r:id="rId74" display="https://www.doi.org/10.5281/zenodo.8173703"/>
+    <hyperlink ref="L22" r:id="rId75" display="https://doi.org/10.48550/arXiv.2203.15395"/>
+    <hyperlink ref="R22" r:id="rId76" display="https://openreview.net/forum?id=N9Wn91tE7D0"/>
+    <hyperlink ref="I23" r:id="rId77" display="https://arxiv.org/abs/2204.11830"/>
+    <hyperlink ref="J23" r:id="rId78" display="https://www.doi.org/10.5281/zenodo.8173705"/>
+    <hyperlink ref="L23" r:id="rId79" display="https://doi.org/10.48550/arXiv.2204.11830"/>
+    <hyperlink ref="R23" r:id="rId80" display="https://openreview.net/forum?id=a_9YF58u61"/>
+    <hyperlink ref="I24" r:id="rId81" display="https://openreview.net/forum?id=irARV_2VFs4"/>
+    <hyperlink ref="J24" r:id="rId82" display="https://www.doi.org/10.5281/zenodo.8173707"/>
+    <hyperlink ref="L24" r:id="rId83" display="https://doi.org/10.48550/arXiv.2110.02619"/>
+    <hyperlink ref="R24" r:id="rId84" display="https://openreview.net/forum?id=ye8PftiQLQ"/>
+    <hyperlink ref="I25" r:id="rId85" display="https://arxiv.org/abs/2203.01928"/>
+    <hyperlink ref="J25" r:id="rId86" display="https://www.doi.org/10.5281/zenodo.8173711"/>
+    <hyperlink ref="L25" r:id="rId87" display="https://doi.org/10.48550/arXiv.2203.01928"/>
+    <hyperlink ref="R25" r:id="rId88" display="https://openreview.net/forum?id=n2qXFXiMsAM"/>
+    <hyperlink ref="I26" r:id="rId89" display="https://ieeexplore.ieee.org/document/9878481"/>
+    <hyperlink ref="J26" r:id="rId90" display="https://www.doi.org/10.5281/zenodo.8173713"/>
+    <hyperlink ref="R26" r:id="rId91" display="https://openreview.net/forum?id=nsrHznwHhl"/>
+    <hyperlink ref="I27" r:id="rId92" display="https://openaccess.thecvf.com/content/CVPR2022/papers/Hirota_Quantifying_Societal_Bias_Amplification_in_Image_Captioning_CVPR_2022_paper.pdf"/>
+    <hyperlink ref="J27" r:id="rId93" display="https://www.doi.org/10.5281/zenodo.8173715"/>
+    <hyperlink ref="R27" r:id="rId94" display="https://openreview.net/forum?id=eJmQJT0Dtt"/>
+    <hyperlink ref="I28" r:id="rId95" display="https://ojs.aaai.org/index.php/AAAI/article/view/21454"/>
+    <hyperlink ref="J28" r:id="rId96" display="https://www.doi.org/10.5281/zenodo.8173717"/>
+    <hyperlink ref="L28" r:id="rId97" display="https://doi.org/10.1609/aaai.v36i11.21454"/>
+    <hyperlink ref="R28" r:id="rId98" display="https://openreview.net/forum?id=WnaVgRhlyT"/>
+    <hyperlink ref="I29" r:id="rId99" display="https://arxiv.org/abs/2106.03761v4"/>
+    <hyperlink ref="J29" r:id="rId100" display="https://www.doi.org/10.5281/zenodo.8173719"/>
+    <hyperlink ref="L29" r:id="rId101" display="https://doi.org/10.48550/arXiv.2106.03761"/>
+    <hyperlink ref="R29" r:id="rId102" display="https://openreview.net/forum?id=jDBYRwDpeW"/>
+    <hyperlink ref="I30" r:id="rId103" display="https://www.ecva.net/papers/eccv_2022/papers_ECCV/papers/136720439.pdf"/>
+    <hyperlink ref="J30" r:id="rId104" display="https://www.doi.org/10.5281/zenodo.8173721"/>
+    <hyperlink ref="R30" r:id="rId105" display="https://openreview.net/forum?id=DWKJpl8s06"/>
+    <hyperlink ref="I31" r:id="rId106" display="https://arxiv.org/abs/2111.13650v3"/>
+    <hyperlink ref="J31" r:id="rId107" display="https://www.doi.org/10.5281/zenodo.8173725"/>
+    <hyperlink ref="L31" r:id="rId108" display="https://doi.org/10.48550/arXiv.2111.13650"/>
+    <hyperlink ref="R31" r:id="rId109" display="https://openreview.net/forum?id=J-Lgb7Vc0wX"/>
+    <hyperlink ref="I32" r:id="rId110" display="https://arxiv.org/abs/2201.12360"/>
+    <hyperlink ref="J32" r:id="rId111" display="https://www.doi.org/10.5281/zenodo.8173729"/>
+    <hyperlink ref="L32" r:id="rId112" display="https://doi.org/10.48550/arXiv.2201.12360"/>
+    <hyperlink ref="R32" r:id="rId113" display="https://openreview.net/forum?id=d7-ns6SZqp"/>
+    <hyperlink ref="I33" r:id="rId114" display="https://ojs.aaai.org/index.php/AAAI/article/view/16721"/>
+    <hyperlink ref="J33" r:id="rId115" display="https://www.doi.org/10.5281/zenodo.8173733"/>
+    <hyperlink ref="L33" r:id="rId116" display="https://doi.org/10.1609/aaai.v35i6.16721"/>
+    <hyperlink ref="R33" r:id="rId117" display="https://openreview.net/forum?id=vWzZQAahuW"/>
+    <hyperlink ref="I34" r:id="rId118" display="https://aclanthology.org/2022.naacl-main.401.pdf"/>
+    <hyperlink ref="J34" r:id="rId119" display="https://www.doi.org/10.5281/zenodo.8173735"/>
+    <hyperlink ref="L34" r:id="rId120" display="https://doi.org/10.48550/arXiv.2204.06305"/>
+    <hyperlink ref="R34" r:id="rId121" display="https://openreview.net/forum?id=t8ZZ2Y356Ix"/>
+    <hyperlink ref="I35" r:id="rId122" display="https://proceedings.mlr.press/v162/han22c.html"/>
+    <hyperlink ref="J35" r:id="rId123" display="https://www.doi.org/10.5281/zenodo.8173737"/>
+    <hyperlink ref="L35" r:id="rId124" display="https://doi.org/10.48550/arXiv.2202.07179"/>
+    <hyperlink ref="R35" r:id="rId125" display="https://openreview.net/forum?id=T54wy0ahGLG&amp;noteId=pvukxfvJGX"/>
+    <hyperlink ref="I36" r:id="rId126" display="https://dl.acm.org/doi/pdf/10.1145/3531146.3533144"/>
+    <hyperlink ref="J36" r:id="rId127" display="https://www.doi.org/10.5281/zenodo.8173739"/>
+    <hyperlink ref="L36" r:id="rId128" display="https://doi.org/10.1145/3531146.3533144"/>
+    <hyperlink ref="R36" r:id="rId129" display="https://openreview.net/forum?id=MjZVx7a0KX-"/>
+    <hyperlink ref="I37" r:id="rId130" display="https://arxiv.org/abs/2203.15395"/>
+    <hyperlink ref="J37" r:id="rId131" display="https://www.doi.org/10.5281/zenodo.8173741"/>
+    <hyperlink ref="L37" r:id="rId132" display="https://doi.org/10.48550/arXiv.2203.15395"/>
+    <hyperlink ref="R37" r:id="rId133" display="https://openreview.net/forum?id=9_hCoP3LXwy"/>
+    <hyperlink ref="I38" r:id="rId134" display="https://openreview.net/forum?id=OIs3SxU5Ynl"/>
+    <hyperlink ref="J38" r:id="rId135" display="https://www.doi.org/10.5281/zenodo.8173745"/>
+    <hyperlink ref="L38" r:id="rId136" display="https://doi.org/10.48550/arXiv.2102.09310"/>
+    <hyperlink ref="R38" r:id="rId137" display="https://openreview.net/forum?id=ozbAwipuZu"/>
+    <hyperlink ref="I39" r:id="rId138" display="https://arxiv.org/pdf/2105.02725.pdf"/>
+    <hyperlink ref="J39" r:id="rId139" display="https://www.doi.org/10.5281/zenodo.8173747"/>
+    <hyperlink ref="L39" r:id="rId140" display="https://doi.org/10.1609/aaai.v36i11.21454"/>
+    <hyperlink ref="R39" r:id="rId141" display="https://openreview.net/forum?id=KNp7Zq3KkT0&amp;noteId=xqiAvezWIN"/>
+    <hyperlink ref="I40" r:id="rId142" display="https://arxiv.org/abs/2105.02725"/>
+    <hyperlink ref="J40" r:id="rId143" display="https://www.doi.org/10.5281/zenodo.8173749"/>
+    <hyperlink ref="L40" r:id="rId144" display="https://doi.org/10.48550/arXiv.2105.02725"/>
+    <hyperlink ref="R40" r:id="rId145" display="https://openreview.net/forum?id=tpk45Zll8eh"/>
+    <hyperlink ref="I41" r:id="rId146" display="https://openaccess.thecvf.com/content/CVPR2022/html/He_Masked_Autoencoders_Are_Scalable_Vision_Learners_CVPR_2022_paper.html"/>
+    <hyperlink ref="J41" r:id="rId147" display="https://www.doi.org/10.5281/zenodo.8173751"/>
+    <hyperlink ref="R41" r:id="rId148" display="https://openreview.net/forum?id=KXfjZPL5pqr"/>
+    <hyperlink ref="I42" r:id="rId149" display="https://proceedings.mlr.press/v139/yuan21c"/>
+    <hyperlink ref="J42" r:id="rId150" display="https://www.doi.org/10.5281/zenodo.8173753"/>
+    <hyperlink ref="L42" r:id="rId151" display="https://doi.org/10.48550/arXiv.2102.05152"/>
+    <hyperlink ref="R42" r:id="rId152" display="https://openreview.net/forum?id=zKBJw4Ht8s"/>
+    <hyperlink ref="I43" r:id="rId153" display="https://openreview.net/pdf?id=6at6rB3IZm"/>
+    <hyperlink ref="J43" r:id="rId154" display="https://www.doi.org/10.5281/zenodo.8173755"/>
+    <hyperlink ref="L43" r:id="rId155" display="https://doi.org/10.48550/arXiv.2205.10343"/>
+    <hyperlink ref="R43" r:id="rId156" display="https://openreview.net/forum?id=Vz9VLcJqKS"/>
+    <hyperlink ref="I44" r:id="rId157" display="https://proceedings.neurips.cc/paper_files/paper/2022/hash/90d17e882adbdda42349db6f50123817-Abstract-Conference.html"/>
+    <hyperlink ref="J44" r:id="rId158" display="https://www.doi.org/10.5281/zenodo.8173757"/>
+    <hyperlink ref="L44" r:id="rId159" display="https://doi.org/10.48550/arXiv.2206.11251"/>
+    <hyperlink ref="R44" r:id="rId160" display="https://openreview.net/forum?id=E0qO5dI5aEn"/>
+    <hyperlink ref="I45" r:id="rId161" display="https://aclanthology.org/2021.acl-long.75/"/>
+    <hyperlink ref="J45" r:id="rId162" display="https://www.doi.org/10.5281/zenodo.8173759"/>
+    <hyperlink ref="R45" r:id="rId163" display="https://openreview.net/forum?id=MF9uv95psps"/>
+    <hyperlink ref="I46" r:id="rId164" display="https://proceedings.mlr.press/v162/zada22a"/>
+    <hyperlink ref="J46" r:id="rId165" display="https://www.doi.org/10.5281/zenodo.8173763"/>
+    <hyperlink ref="L46" r:id="rId166" display="https://doi.org/10.48550/arXiv.2112.08810"/>
+    <hyperlink ref="R46" r:id="rId167" display="https://openreview.net/forum?id=ErBe4MnsVD"/>
+    <hyperlink ref="G47" r:id="rId168" display="https://zenodo.org/record/6574723/files/article.pdf"/>
+    <hyperlink ref="G48" r:id="rId169" display="https://zenodo.org/record/6574625/files/article.pdf"/>
+    <hyperlink ref="H48" r:id="rId170" display="https://github.com/ambekarsameer96/FACT_AI/"/>
+    <hyperlink ref="I48" r:id="rId171" display="https://arxiv.org/abs/2101.06046"/>
+    <hyperlink ref="L48" r:id="rId172" display="https://doi.org/10.48550/arXiv.2101.06046"/>
+    <hyperlink ref="R48" r:id="rId173" display="https://openreview.net/forum?id=BSHg22G7n0F"/>
+    <hyperlink ref="G49" r:id="rId174" display="https://zenodo.org/record/6574629/files/article.pdf"/>
+    <hyperlink ref="H49" r:id="rId175" display="https://github.com/ashok-arjun/MLRC-2021-Few-Shot-Learning-And-Self-Supervision/"/>
+    <hyperlink ref="I49" r:id="rId176" display="https://openreview.net/forum?id=738x44N7yUE&amp;noteId=46xr8OHtA-"/>
+    <hyperlink ref="L49" r:id="rId177" display="https://doi.org/10.48550/arXiv.1910.03560"/>
+    <hyperlink ref="R49" r:id="rId178" display="https://openreview.net/forum?id=ScfP3G73CY"/>
+    <hyperlink ref="G50" r:id="rId179" display="https://zenodo.org/record/6574631/files/article.pdf"/>
+    <hyperlink ref="H50" r:id="rId180" display="https://github.com/athaioan/ViT_Affinity_Reproducibility_Challenge"/>
+    <hyperlink ref="I50" r:id="rId181" display="https://openaccess.thecvf.com/content/CVPR2021/papers/Chefer_Transformer_Interpretability_Beyond_Attention_Visualization_CVPR_2021_paper.pdf"/>
+    <hyperlink ref="R50" r:id="rId182" display="https://openreview.net/forum?id=rcEDhGX3AY"/>
+    <hyperlink ref="G51" r:id="rId183" display="https://zenodo.org/record/6574635/files/article.pdf"/>
+    <hyperlink ref="H51" r:id="rId184" display="https://github.com/danilodegoede/fact-team3/"/>
+    <hyperlink ref="I51" r:id="rId185" display="https://openreview.net/pdf?id=BXewfAYMmJw"/>
+    <hyperlink ref="L51" r:id="rId186" display="https://doi.org/10.48550/arXiv.2101.06046"/>
+    <hyperlink ref="R51" r:id="rId187" display="https://openreview.net/forum?id=HNlzT3G720t"/>
+    <hyperlink ref="G52" r:id="rId188" display="https://zenodo.org/record/6574637/files/article.pdf"/>
+    <hyperlink ref="H52" r:id="rId189" display="https://github.com/reproducibilityaccount/reproducing-ridesharing"/>
+    <hyperlink ref="I52" r:id="rId190" display="https://www.ijcai.org/proceedings/2021/51 "/>
+    <hyperlink ref="L52" r:id="rId191" display="https://doi.org/10.24963/ijcai.2021/51"/>
+    <hyperlink ref="R52" r:id="rId192" display="https://openreview.net/forum?id=BE3Ms3GXhCF"/>
+    <hyperlink ref="G53" r:id="rId193" display="https://zenodo.org/record/6574639/files/article.pdf"/>
+    <hyperlink ref="H53" r:id="rId194" display="https://github.com/matteobrv/repro-SKS"/>
+    <hyperlink ref="I53" r:id="rId195" display="https://aclanthology.org/2021.acl-long.556.pdf"/>
+    <hyperlink ref="R53" r:id="rId196" display="https://openreview.net/forum?id=SSSGs3M7nRY"/>
+    <hyperlink ref="G54" r:id="rId197" display="https://zenodo.org/record/6574641/files/article.pdf"/>
+    <hyperlink ref="H54" r:id="rId198" display="https://github.com/kayatb/reproduce_SCOUTER"/>
+    <hyperlink ref="I54" r:id="rId199" display="https://openaccess.thecvf.com/content/ICCV2021/html/Li_SCOUTER_Slot_Attention-Based_Classifier_for_Explainable_Image_Recognition_ICCV_2021_paper.html"/>
+    <hyperlink ref="R54" r:id="rId200" display="https://openreview.net/forum?id=HZNlq3fmhRF"/>
+    <hyperlink ref="G55" r:id="rId201" display="https://zenodo.org/record/6574643/files/article.pdf"/>
+    <hyperlink ref="H55" r:id="rId202" display="https://github.com/anirudhb11/Adabelief-Optimizer-RC"/>
+    <hyperlink ref="I55" r:id="rId203" display="https://openreview.net/forum?id=YeSwJDOnTRY&amp;referrer=%5BML%20Reproducibility%20Challenge%202021%20Spring%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2021%2FSpring)"/>
+    <hyperlink ref="L55" r:id="rId204" display="https://doi.org/10.48550/arXiv.2010.07468"/>
+    <hyperlink ref="R55" r:id="rId205" display="https://openreview.net/forum?id=B9gDnMmn0t"/>
+    <hyperlink ref="G56" r:id="rId206" display="https://zenodo.org/record/6574645/files/article.pdf"/>
+    <hyperlink ref="H56" r:id="rId207" display="https://github.com/midsterx/ReGANSpace"/>
+    <hyperlink ref="I56" r:id="rId208" display="https://openreview.net/forum?id=WCRIASdNpsR&amp;noteId=geUtL2j1uoH"/>
+    <hyperlink ref="L56" r:id="rId209" display="https://doi.org/10.48550/arXiv.2004.02546"/>
+    <hyperlink ref="R56" r:id="rId210" display="https://openreview.net/forum?id=BtZVD2f7n0F"/>
+    <hyperlink ref="G57" r:id="rId211" display="https://zenodo.org/record/6574647/files/article.pdf"/>
+    <hyperlink ref="H57" r:id="rId212" display="https://github.com/stfwn/ats-privacy-replication"/>
+    <hyperlink ref="I57" r:id="rId213" display="https://openaccess.thecvf.com/content/CVPR2021/papers/Gao_Privacy-Preserving_Collaborative_Learning_With_Automatic_Transformation_Search_CVPR_2021_paper.pdf"/>
+    <hyperlink ref="R57" r:id="rId214" display="https://openreview.net/forum?id=SY84JTG73CK"/>
+    <hyperlink ref="G58" r:id="rId215" display="https://zenodo.org/record/6574649/files/article.pdf"/>
+    <hyperlink ref="H58" r:id="rId216" display="https://github.com/Benidzu/isotropy_reproduction"/>
+    <hyperlink ref="I58" r:id="rId217" display="https://aclanthology.org/2021.acl-short.73.pdf"/>
+    <hyperlink ref="R58" r:id="rId218" display="https://openreview.net/forum?id=rxWeB3zQ2CY"/>
+    <hyperlink ref="G59" r:id="rId219" display="https://zenodo.org/record/6574651/files/article.pdf"/>
+    <hyperlink ref="H59" r:id="rId220" display="https://github.com/Pnaghavi/Mitigating-Gender-Bias-in-Generated-Text"/>
+    <hyperlink ref="I59" r:id="rId221" display="https://aclanthology.org/2020.emnlp-main.656"/>
+    <hyperlink ref="R59" r:id="rId222" display="https://openreview.net/forum?id=StblE2MQ3AY"/>
+    <hyperlink ref="G60" r:id="rId223" display="https://zenodo.org/record/6574653/files/article.pdf"/>
+    <hyperlink ref="H60" r:id="rId224" display="https://github.com/MarkiemarkF/FACT"/>
+    <hyperlink ref="I60" r:id="rId225" display="https://ojs.aaai.org/index.php/AAAI/article/view/17336"/>
+    <hyperlink ref="L60" r:id="rId226" display="https://doi.org/10.1609/aaai.v35i12.17336"/>
+    <hyperlink ref="R60" r:id="rId227" display="https://openreview.net/forum?id=rq8fRhMm20F"/>
+    <hyperlink ref="G61" r:id="rId228" display="https://zenodo.org/record/6574655/files/article.pdf"/>
+    <hyperlink ref="H61" r:id="rId229" display="https://github.com/irenepap2/Re_StylEx.git"/>
+    <hyperlink ref="I61" r:id="rId230" display="https://openaccess.thecvf.com/content/ICCV2021/papers/Lang_Explaining_in_Style_Training_a_GAN_To_Explain_a_Classifier_ICCV_2021_paper.pdf"/>
+    <hyperlink ref="R61" r:id="rId231" display="https://openreview.net/forum?id=SK8gAhfX2AK"/>
+    <hyperlink ref="G62" r:id="rId232" display="https://zenodo.org/record/6574657/files/article.pdf"/>
+    <hyperlink ref="H62" r:id="rId233" display="https://github.com/Ian-Hardy/Fair_Robust_Modeling"/>
+    <hyperlink ref="I62" r:id="rId234" display="https://arxiv.org/pdf/2010.06121.pdf"/>
+    <hyperlink ref="L62" r:id="rId235" display="https://doi.org/10.48550/arXiv.2010.06121"/>
+    <hyperlink ref="R62" r:id="rId236" display="https://openreview.net/forum?id=Sczshz7h0K"/>
+    <hyperlink ref="G63" r:id="rId237" display="https://zenodo.org/record/6574659/files/article.pdf"/>
+    <hyperlink ref="H63" r:id="rId238" display="https://github.com/miszkur/SelfSupervisedLearning"/>
+    <hyperlink ref="I63" r:id="rId239" display="http://proceedings.mlr.press/v139/tian21a/tian21a.pdf"/>
+    <hyperlink ref="L63" r:id="rId240" display="https://doi.org/10.48550/arXiv.2102.06810"/>
+    <hyperlink ref="R63" r:id="rId241" display="https://openreview.net/forum?id=r4xe3nMQ3AY"/>
+    <hyperlink ref="G64" r:id="rId242" display="https://zenodo.org/record/6574661/files/article.pdf"/>
+    <hyperlink ref="H64" r:id="rId243" display="https://github.com/rjiles/causalmatching"/>
+    <hyperlink ref="I64" r:id="rId244" display="https://arxiv.org/pdf/2006.07500.pdf"/>
+    <hyperlink ref="L64" r:id="rId245" display="https://doi.org/10.48550/arXiv.2006.07500"/>
+    <hyperlink ref="R64" r:id="rId246" display="https://openreview.net/forum?id=r43elaGmhCY"/>
+    <hyperlink ref="G65" r:id="rId247" display="https://zenodo.org/record/6574663/files/article.pdf"/>
+    <hyperlink ref="H65" r:id="rId248" display="https://github.com/DCHamerslag/FACT"/>
+    <hyperlink ref="I65" r:id="rId249" display="https://arxiv.org/pdf/2012.08723.pdf"/>
+    <hyperlink ref="L65" r:id="rId250" display="https://doi.org/10.48550/arXiv.2012.08723"/>
+    <hyperlink ref="R65" r:id="rId251" display="https://openreview.net/forum?id=rKbgh3fXnRK"/>
+    <hyperlink ref="G66" r:id="rId252" display="https://zenodo.org/record/6574665/files/article.pdf"/>
+    <hyperlink ref="H66" r:id="rId253" display="https://github.com/GuillyK/FACT-ai"/>
+    <hyperlink ref="I66" r:id="rId254" display="https://arxiv.org/pdf/2103.01826.pdf"/>
+    <hyperlink ref="L66" r:id="rId255" display="https://doi.org/10.48550/arXiv.2103.01826"/>
+    <hyperlink ref="R66" r:id="rId256" display="https://openreview.net/forum?id=rNgg03fXnRY"/>
+    <hyperlink ref="G67" r:id="rId257" display="https://zenodo.org/record/6574667/files/article.pdf"/>
+    <hyperlink ref="H67" r:id="rId258" display="https://github.com/Gijsvanmeer/FACTinAI"/>
+    <hyperlink ref="I67" r:id="rId259" display="https://arxiv.org/abs/2104.13369"/>
+    <hyperlink ref="L67" r:id="rId260" display="https://doi.org/10.48550/arXiv.2104.13369"/>
+    <hyperlink ref="R67" r:id="rId261" display="https://openreview.net/forum?id=BtIz0nz7hRY"/>
+    <hyperlink ref="G68" r:id="rId262" display="https://zenodo.org/record/6574669/files/article.pdf"/>
+    <hyperlink ref="H68" r:id="rId263" display="https://github.com/imandrealombardo/FACT-AI"/>
+    <hyperlink ref="I68" r:id="rId264" display="https://ojs.aaai.org/index.php/AAAI/article/view/17080"/>
+    <hyperlink ref="L68" r:id="rId265" display="https://doi.org/10.1609/aaai.v35i10.17080"/>
+    <hyperlink ref="R68" r:id="rId266" display="https://openreview.net/forum?id=H4lzChGmhCK"/>
+    <hyperlink ref="G69" r:id="rId267" display="https://zenodo.org/record/6574671/files/article.pdf"/>
+    <hyperlink ref="H69" r:id="rId268" display="https://github.com/andrazdeluisa/reproducibility_challenge"/>
+    <hyperlink ref="I69" r:id="rId269" display="https://www.ijcai.org/proceedings/2021/0305.pdf"/>
+    <hyperlink ref="R69" r:id="rId270" display="https://openreview.net/forum?id=r5LS3fmh0t"/>
+    <hyperlink ref="G70" r:id="rId271" display="https://zenodo.org/record/6574673/files/article.pdf"/>
+    <hyperlink ref="H70" r:id="rId272" display="https://github.com/Di-ayy-go/fact-ai"/>
+    <hyperlink ref="I70" r:id="rId273" display="https://proceedings.mlr.press/v139/correa21a"/>
+    <hyperlink ref="R70" r:id="rId274" display="https://openreview.net/forum?id=SNeep2MXn0K"/>
+    <hyperlink ref="G71" r:id="rId275" display="https://zenodo.org/record/6574675/files/article.pdf"/>
+    <hyperlink ref="H71" r:id="rId276" display="https://github.com/andyzfchen/truncatedSVD"/>
+    <hyperlink ref="I71" r:id="rId277" display="https://icml.cc/virtual/2021/spotlight/10160"/>
+    <hyperlink ref="R71" r:id="rId278" display="https://openreview.net/forum?id=HN2xWpMQ30K"/>
+    <hyperlink ref="G72" r:id="rId279" display="https://zenodo.org/record/6574677/files/article.pdf"/>
+    <hyperlink ref="H72" r:id="rId280" display="https://github.com/karan-uppal3/BANA"/>
+    <hyperlink ref="I72" r:id="rId281" display="http://openaccess.thecvf.com//content/CVPR2021/papers/Oh_Background-Aware_Pooling_and_Noise-Aware_Loss_for_Weakly-Supervised_Semantic_Segmentation_CVPR_2021_paper.pdf"/>
+    <hyperlink ref="R72" r:id="rId282" display="https://openreview.net/forum?id=rUQllTGQhAY"/>
+    <hyperlink ref="G73" r:id="rId283" display="https://zenodo.org/record/6574679/files/article.pdf"/>
+    <hyperlink ref="H73" r:id="rId284" display="https://github.com/gahaalt/reproducing-comparing-rewinding-and-finetuning"/>
+    <hyperlink ref="I73" r:id="rId285" display="https://openreview.net/forum?id=YrKu2s0HaG6Q&amp;noteId=SxQ0jqm5O0w"/>
+    <hyperlink ref="L73" r:id="rId286" display="https://doi.org/10.1609/aaai.v35i10.17080"/>
+    <hyperlink ref="R73" r:id="rId287" display="https://openreview.net/forum?id=HxWEL2zQ3AK"/>
+    <hyperlink ref="G74" r:id="rId288" display="https://zenodo.org/record/6574681/files/article.pdf"/>
+    <hyperlink ref="H74" r:id="rId289" display="https://github.com/toliz/fairness-attacks"/>
+    <hyperlink ref="I74" r:id="rId290" display="https://ojs.aaai.org/index.php/AAAI/article/view/17080"/>
+    <hyperlink ref="L74" r:id="rId291" display="https://doi.org/10.24963/ijcai.2021/51"/>
+    <hyperlink ref="R74" r:id="rId292" display="https://openreview.net/forum?id=rYLMJ6zX3RF"/>
+    <hyperlink ref="G75" r:id="rId293" display="https://zenodo.org/record/6574683/files/article.pdf"/>
+    <hyperlink ref="H75" r:id="rId294" display="https://github.com/Veranep/rideshare-replication"/>
+    <hyperlink ref="I75" r:id="rId295" display="https://www.ijcai.org/proceedings/2021/51"/>
+    <hyperlink ref="L75" r:id="rId296" display="https://doi.org/10.48550/arXiv.2011.00844"/>
+    <hyperlink ref="R75" r:id="rId297" display="https://openreview.net/forum?id=BEhgn2zm3CK"/>
+    <hyperlink ref="G76" r:id="rId298" display="https://zenodo.org/record/6574685/files/article.pdf"/>
+    <hyperlink ref="H76" r:id="rId299" display="https://github.com/alessioGalatolo/GAN-2D-to-3D"/>
+    <hyperlink ref="I76" r:id="rId300" display="https://openreview.net/forum?id=FGqiDsBUKL0"/>
+    <hyperlink ref="L76" r:id="rId301" display="https://doi.org/10.48550/arXiv.2003.02389"/>
+    <hyperlink ref="R76" r:id="rId302" display="https://openreview.net/forum?id=B8mxkTzX2RY"/>
+    <hyperlink ref="G77" r:id="rId303" display="https://zenodo.org/record/6574687/files/article.pdf"/>
+    <hyperlink ref="H77" r:id="rId304" display="https://github.com/AIExL/vav_rc2021"/>
+    <hyperlink ref="I77" r:id="rId305" display="https://icml.cc/Conferences/2021/Schedule?showEvent=9548"/>
+    <hyperlink ref="L77" r:id="rId306" display="https://doi.org/10.48550/arXiv.2012.01557"/>
+    <hyperlink ref="R77" r:id="rId307" display="https://openreview.net/forum?id=BFLM3nMmhCt"/>
+    <hyperlink ref="G78" r:id="rId308" display="https://zenodo.org/record/6574689/files/article.pdf"/>
+    <hyperlink ref="H78" r:id="rId309" display="https://github.com/pimpraat/FACT-Ai"/>
+    <hyperlink ref="I78" r:id="rId310" display="https://proceedings.mlr.press/v139/correa21a.html"/>
+    <hyperlink ref="R78" r:id="rId311" display="https://openreview.net/forum?id=S9gs3MmhAY"/>
+    <hyperlink ref="G79" r:id="rId312" display="https://zenodo.org/record/6574691/files/article.pdf"/>
+    <hyperlink ref="H79" r:id="rId313" display="https://github.com/MLRC2022FSCS/FSCS"/>
+    <hyperlink ref="I79" r:id="rId314" display="http://proceedings.mlr.press/v139/lee21b.html"/>
+    <hyperlink ref="R79" r:id="rId315" display="https://openreview.net/forum?id=r9Leh2M7hCt"/>
+    <hyperlink ref="G80" r:id="rId316" display="https://zenodo.org/record/6574693/files/article.pdf"/>
+    <hyperlink ref="H80" r:id="rId317" display="https://github.com/sirmisscriesalot/Differentiable-Spatial-Planning-using-Transformers"/>
+    <hyperlink ref="I80" r:id="rId318" display="http://proceedings.mlr.press/v139/chaplot21a.html"/>
+    <hyperlink ref="L80" r:id="rId319" display="https://doi.org/10.48550/arXiv.2112.01010"/>
+    <hyperlink ref="R80" r:id="rId320" display="https://openreview.net/forum?id=HFUI1pfQnCF"/>
+    <hyperlink ref="G81" r:id="rId321" display="https://zenodo.org/record/6574695/files/article.pdf"/>
+    <hyperlink ref="H81" r:id="rId322" display="https://github.com/tuelwer/machine-learning-reproducibility-challenge-2021"/>
+    <hyperlink ref="I81" r:id="rId323" display="https://openreview.net/forum?id=aGfr4iF_Li&amp;noteId=dOsxraq3Vto"/>
+    <hyperlink ref="L81" r:id="rId324" display="https://doi.org/10.48550/arXiv.2007.14621"/>
+    <hyperlink ref="R81" r:id="rId325" display="https://openreview.net/forum?id=rlWzUnM72RF"/>
+    <hyperlink ref="G82" r:id="rId326" display="https://zenodo.org/record/6574697/files/article.pdf"/>
+    <hyperlink ref="H82" r:id="rId327" display="https://github.com/RoopsaSen/social-nce-trajectron-plus-plus"/>
+    <hyperlink ref="I82" r:id="rId328" display="https://openaccess.thecvf.com/content/ICCV2021/papers/Liu_Social_NCE_Contrastive_Learning_of_Socially-Aware_Motion_Representations_ICCV_2021_paper.pdf"/>
+    <hyperlink ref="R82" r:id="rId329" display="https://openreview.net/forum?id=SIQEl6f7h0Y"/>
+    <hyperlink ref="G83" r:id="rId330" display="https://zenodo.org/record/6574699/files/article.pdf"/>
+    <hyperlink ref="H83" r:id="rId331" display="https://github.com/Viswesh-N/MLRC-2021"/>
+    <hyperlink ref="I83" r:id="rId332" display="https://arxiv.org/abs/2012.01526"/>
+    <hyperlink ref="L83" r:id="rId333" display="https://doi.org/10.48550/arXiv.2012.01526"/>
+    <hyperlink ref="R83" r:id="rId334" display="https://openreview.net/forum?id=HV2zgpM7n0F"/>
+    <hyperlink ref="G84" r:id="rId335" display="https://zenodo.org/record/6574701/files/article.pdf"/>
+    <hyperlink ref="H84" r:id="rId336" display="https://github.com/MarusaOrazem/reproducibility_challenge"/>
+    <hyperlink ref="I84" r:id="rId337" display="https://openreview.net/forum?id=dlEJsyHGeaL"/>
+    <hyperlink ref="R84" r:id="rId338" display="https://openreview.net/forum?id=H5lOnzXhAY"/>
+    <hyperlink ref="G85" r:id="rId339" display="https://zenodo.org/record/6574703/files/article.pdf"/>
+    <hyperlink ref="H85" r:id="rId340" display="https://github.com/tersekmatija/re-LearningToCountEverything"/>
+    <hyperlink ref="I85" r:id="rId341" display="https://openaccess.thecvf.com/content/CVPR2021/html/Ranjan_Learning_To_Count_Everything_CVPR_2021_paper.html"/>
+    <hyperlink ref="R85" r:id="rId342" display="https://openreview.net/forum?id=HKbgd3zmh0t"/>
+    <hyperlink ref="G86" r:id="rId343" display="https://zenodo.org/record/6574705/files/article.pdf"/>
+    <hyperlink ref="H86" r:id="rId344" display="https://github.com/thesofakillers/badder-seeds"/>
+    <hyperlink ref="I86" r:id="rId345" display="https://aclanthology.org/2021.acl-long.148/"/>
+    <hyperlink ref="R86" r:id="rId346" display="https://openreview.net/forum?id=HcIxA3Mm2CF"/>
+    <hyperlink ref="G87" r:id="rId347" display="https://zenodo.org/record/6574707/files/article.pdf"/>
+    <hyperlink ref="H87" r:id="rId348" display="https://github.com/trojerz/TOTB-reproducability"/>
+    <hyperlink ref="I87" r:id="rId349" display="https://openaccess.thecvf.com/content/ICCV2021/papers/Fan_Transparent_Object_Tracking_Benchmark_ICCV_2021_paper.pdf"/>
+    <hyperlink ref="R87" r:id="rId350" display="https://openreview.net/forum?id=HxZZV3MQ20Y"/>
+    <hyperlink ref="G88" r:id="rId351" display="https://zenodo.org/record/6574709/files/article.pdf"/>
+    <hyperlink ref="H88" r:id="rId352" display="https://github.com/NoahVl/Explaining-In-Style-Reproducibility-Study"/>
+    <hyperlink ref="I88" r:id="rId353" display="https://openaccess.thecvf.com/content/ICCV2021/papers/Lang_Explaining_in_Style_Training_a_GAN_To_Explain_a_Classifier_ICCV_2021_paper.pdf"/>
+    <hyperlink ref="R88" r:id="rId354" display="https://openreview.net/forum?id=SYUxyazQh0Y"/>
+    <hyperlink ref="G89" r:id="rId355" display="https://zenodo.org/record/6574711/files/article.pdf"/>
+    <hyperlink ref="H89" r:id="rId356" display="https://github.com/ShuaiWang97/UvA_FACT2022"/>
+    <hyperlink ref="I89" r:id="rId357" display="https://openreview.net/forum?id=XN1M27T6uux"/>
+    <hyperlink ref="L89" r:id="rId358" display="https://doi.org/10.48550/arXiv.2110.12884"/>
+    <hyperlink ref="R89" r:id="rId359" display="https://openreview.net/forum?id=SVx46hzmhRK"/>
+    <hyperlink ref="G90" r:id="rId360" display="https://zenodo.org/record/6574713/files/article.pdf"/>
+    <hyperlink ref="H90" r:id="rId361" display="https://github.com/Linkerbrain/fact-ai-2021-project"/>
+    <hyperlink ref="I90" r:id="rId362" display="https://openaccess.thecvf.com/content/CVPR2021/html/Gao_Privacy-Preserving_Collaborative_Learning_With_Automatic_Transformation_Search_CVPR_2021_paper.html"/>
+    <hyperlink ref="R90" r:id="rId363" display="https://openreview.net/forum?id=S9Iepnz7hRY"/>
+    <hyperlink ref="G91" r:id="rId364" display="https://zenodo.org/record/6574715/files/article.pdf"/>
+    <hyperlink ref="H91" r:id="rId365" display="https://github.com/RomanOort/FACTAI"/>
+    <hyperlink ref="I91" r:id="rId366" display="https://openreview.net/forum?id=wGmOLwb8ClT"/>
+    <hyperlink ref="L91" r:id="rId367" display="https://doi.org/10.48550/arXiv.2107.04086"/>
+    <hyperlink ref="R91" r:id="rId368" display="https://openreview.net/forum?id=HWNgihGX20Y"/>
+    <hyperlink ref="G92" r:id="rId369" display="https://zenodo.org/record/6574719/files/article.pdf"/>
+    <hyperlink ref="H92" r:id="rId370" display="https://github.com/yilmazdoga/lifting-2d-stylegan-for-3d-aware-face-generation"/>
+    <hyperlink ref="I92" r:id="rId371" display="https://openaccess.thecvf.com/content/CVPR2021/papers/Shi_Lifting_2D_StyleGAN_for_3D-Aware_Face_Generation_CVPR_2021_paper.pdf"/>
+    <hyperlink ref="L92" r:id="rId372" display="https://doi.org/10.48550/arXiv.2011.13126"/>
+    <hyperlink ref="R92" r:id="rId373" display="https://openreview.net/forum?id=BcNonfQ3RY"/>
+    <hyperlink ref="G93" r:id="rId374" display="https://zenodo.org/record/6574721/files/article.pdf"/>
+    <hyperlink ref="H93" r:id="rId375" display="https://github.com/zrimseku/Reproducibility-Challenge"/>
+    <hyperlink ref="I93" r:id="rId376" display="https://arxiv.org/pdf/2105.06709.pdf"/>
+    <hyperlink ref="R93" r:id="rId377" display="https://openreview.net/forum?id=Hc8GOhfmhRF"/>
+    <hyperlink ref="G94" r:id="rId378" display="https://zenodo.org/record/6574623/files/article.pdf"/>
+    <hyperlink ref="H94" r:id="rId379" display="https://github.com/wi25hoy/MLRC21_Nondeterminism"/>
+    <hyperlink ref="I94" r:id="rId380" display="https://paperswithcode.com/paper/nondeterminism-and-instability-in-neural"/>
+    <hyperlink ref="L94" r:id="rId381" display="https://doi.org/10.48550/arXiv.2103.04514"/>
+    <hyperlink ref="R94" r:id="rId382" display="https://openreview.net/forum?id=BNefkaG73At"/>
+    <hyperlink ref="G95" r:id="rId383" display="https://zenodo.org/record/4835602/files/article.pdf"/>
+    <hyperlink ref="H95" r:id="rId384" display="https://github.com/elfrink1/FACT"/>
+    <hyperlink ref="I95" r:id="rId385" display="https://openreview.net/forum?id=MFj70_2-eY1&amp;noteId=qf1uS0EEyLy&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L95" r:id="rId386" display="https://doi.org/10.48550/arXiv.2003.01640"/>
+    <hyperlink ref="R95" r:id="rId387" display="https://openreview.net/forum?id=cqAHExg2f"/>
+    <hyperlink ref="G96" r:id="rId388" display="https://zenodo.org/record/4833219/files/article.pdf"/>
+    <hyperlink ref="H96" r:id="rId389" display="https://github.com/tzole1155/EndToEndObjectPose"/>
+    <hyperlink ref="I96" r:id="rId390" display="https://openreview.net/forum?id=fgUXyn4Qrk0&amp;noteId=n4yKe2VVmN3&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L96" r:id="rId391" display="https://doi.org/10.48550/arXiv.1909.06043"/>
+    <hyperlink ref="R96" r:id="rId392" display="https://openreview.net/forum?id=PCpGvUrwfQB"/>
+    <hyperlink ref="G97" r:id="rId393" display="https://zenodo.org/record/4833389/files/article.pdf"/>
+    <hyperlink ref="H97" r:id="rId394" display="https://github.com/mayurak47/Reproducibility_Challenge"/>
+    <hyperlink ref="I97" r:id="rId395" display="https://openreview.net/forum?id=r_qY49Av7wj&amp;noteId=hEN70lsEC4&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L97" r:id="rId396" display="https://doi.org/10.48550/arXiv.2006.08195"/>
+    <hyperlink ref="R97" r:id="rId397" display="https://openreview.net/forum?id=ysFCiXtCOj"/>
+    <hyperlink ref="G98" r:id="rId398" display="https://zenodo.org/record/4833547/files/article.pdf"/>
+    <hyperlink ref="H98" r:id="rId399" display="https://github.com/topteulen/UVA-FACT"/>
+    <hyperlink ref="I98" r:id="rId400" display="https://openreview.net/forum?id=MhMYW2PqGSH"/>
+    <hyperlink ref="R98" r:id="rId401" display="https://openreview.net/forum?id=DXVAJGohUKs"/>
+    <hyperlink ref="G99" r:id="rId402" display="https://zenodo.org/record/4833681/files/article.pdf"/>
+    <hyperlink ref="H99" r:id="rId403" display="https://github.com/prateekstark/training-binary-neural-network"/>
+    <hyperlink ref="I99" r:id="rId404" display="https://openreview.net/forum?id=jsrGMN98wJ&amp;noteId=D7XO0agO1i5&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L99" r:id="rId405" display="https://doi.org/10.48550/arXiv.2002.10778"/>
+    <hyperlink ref="R99" r:id="rId406" display="https://openreview.net/forum?id=bhiGno-Cxq"/>
+    <hyperlink ref="G100" r:id="rId407" display="https://zenodo.org/record/4834146/files/article.pdf"/>
+    <hyperlink ref="H100" r:id="rId408" display="https://github.com/MatPrst/deceptive-attention-reproduced"/>
+    <hyperlink ref="I100" r:id="rId409" display="https://openreview.net/forum?id=ZVxchkVPa8S"/>
+    <hyperlink ref="R100" r:id="rId410" display="https://openreview.net/forum?id=-rn9m0Gt6AQ"/>
+    <hyperlink ref="G101" r:id="rId411" display="https://zenodo.org/record/4834242/files/article.pdf"/>
+    <hyperlink ref="H101" r:id="rId412" display="https://github.com/LarsHoldijk/RE-ParameterizedExplainerForGraphNeuralNetworks"/>
+    <hyperlink ref="I101" r:id="rId413" display="https://openreview.net/forum?id=WsphwsV5hV&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L101" r:id="rId414" display="https://doi.org/10.48550/arXiv.2011.04573"/>
+    <hyperlink ref="R101" r:id="rId415" display="https://openreview.net/forum?id=8JHrucviUf"/>
+    <hyperlink ref="G102" r:id="rId416" display="https://zenodo.org/record/4834352/files/article.pdf"/>
+    <hyperlink ref="H102" r:id="rId417" display="https://github.com/princetonvisualai/ContextualBias"/>
+    <hyperlink ref="I102" r:id="rId418" display="https://openreview.net/forum?id=kqKeIP46EF8&amp;noteId=epbmiUjgl51&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="R102" r:id="rId419" display="https://openreview.net/forum?id=PRXM8-O9PKd"/>
+    <hyperlink ref="G103" r:id="rId420" display="https://zenodo.org/record/4834442/files/article.pdf"/>
+    <hyperlink ref="H103" r:id="rId421" display="https://github.com/Celiali/FixMatch.git"/>
+    <hyperlink ref="I103" r:id="rId422" display="https://openreview.net/forum?id=bleIdqV_-JY"/>
+    <hyperlink ref="L103" r:id="rId423" display="https://doi.org/10.48550/arXiv.2001.07685"/>
+    <hyperlink ref="R103" r:id="rId424" display="https://openreview.net/forum?id=3VXeifKSaTE"/>
+    <hyperlink ref="G104" r:id="rId425" display="https://zenodo.org/record/4834516/files/article.pdf"/>
+    <hyperlink ref="H104" r:id="rId426" display="https://github.com/lennelov/endd-reproduce"/>
+    <hyperlink ref="I104" r:id="rId427" display="https://openreview.net/forum?id=BygSP6Vtvr"/>
+    <hyperlink ref="L104" r:id="rId428" display="https://doi.org/10.48550/arXiv.1905.00076"/>
+    <hyperlink ref="R104" r:id="rId429" display="https://openreview.net/forum?id=p1BXNUcTFsN"/>
+    <hyperlink ref="G105" r:id="rId430" display="https://zenodo.org/record/4834610/files/article.pdf"/>
+    <hyperlink ref="I105" r:id="rId431" display="https://openreview.net/forum?id=Emc_HGRBOHH"/>
+    <hyperlink ref="R105" r:id="rId432" display="https://openreview.net/forum?id=vvLWTXkJ2Zv"/>
+    <hyperlink ref="G106" r:id="rId433" display="https://zenodo.org/record/4834672/files/article.pdf"/>
+    <hyperlink ref="H106" r:id="rId434" display="https://github.com/sami-automatic/SADNet_Replication"/>
+    <hyperlink ref="I106" r:id="rId435" display="https://openreview.net/forum?id=8CJIjwUrbls&amp;noteId=r7GUWB4G6oT"/>
+    <hyperlink ref="R106" r:id="rId436" display="https://openreview.net/forum?id=yiAI9QN9nYt&amp;noteId=SMFjCY6qG8"/>
+    <hyperlink ref="G107" r:id="rId437" display="https://zenodo.org/record/4834744/files/article.pdf"/>
+    <hyperlink ref="H107" r:id="rId438" display="https://github.com/dmizr/phuber"/>
+    <hyperlink ref="I107" r:id="rId439" display="https://openreview.net/forum?id=_yBqU7P7_cn&amp;noteId=TezNrEptzwO"/>
+    <hyperlink ref="R107" r:id="rId440" display="https://openreview.net/forum?id=TM_SgwWJA23"/>
+    <hyperlink ref="G108" r:id="rId441" display="https://zenodo.org/record/4834856/files/article.pdf"/>
+    <hyperlink ref="H108" r:id="rId442" display="https://github.com/CS-433/cs-433-project-2-fesenjoon"/>
+    <hyperlink ref="I108" r:id="rId443" display="https://openreview.net/forum?id=zP0rh1RL8y-"/>
+    <hyperlink ref="L108" r:id="rId444" display="https://doi.org/10.48550/arXiv.1910.08475"/>
+    <hyperlink ref="R108" r:id="rId445" display="https://openreview.net/forum?id=N43DVxrjCw"/>
+    <hyperlink ref="G109" r:id="rId446" display="https://zenodo.org/record/4834942/files/article.pdf"/>
+    <hyperlink ref="H109" r:id="rId447" display="https://github.com/jishnujayakumar/MLRC2020-EmbedKGQA"/>
+    <hyperlink ref="I109" r:id="rId448" display="https://openreview.net/forum?id=PUaAgFaMIlaZ"/>
+    <hyperlink ref="R109" r:id="rId449" display="https://openreview.net/forum?id=VFAwCMdWY7"/>
+    <hyperlink ref="G110" r:id="rId450" display="https://zenodo.org/record/4835056/files/article.pdf"/>
+    <hyperlink ref="H110" r:id="rId451" display="https://github.com/damiaanr/fact-ai"/>
+    <hyperlink ref="I110" r:id="rId452" display="https://openreview.net/forum?id=MFj70_2-eY1"/>
+    <hyperlink ref="L110" r:id="rId453" display="https://doi.org/10.48550/arXiv.2003.01640"/>
+    <hyperlink ref="R110" r:id="rId454" display="https://openreview.net/forum?id=hq3TxQK5cox"/>
+    <hyperlink ref="G111" r:id="rId455" display="https://zenodo.org/record/4839595/files/article.pdf"/>
+    <hyperlink ref="H111" r:id="rId456" display="https://github.com/HiddeLekanne/Reproducibility-Challenge-iFlow"/>
+    <hyperlink ref="I111" r:id="rId457" display="https://openreview.net/forum?id=QxBBSsd_j9b&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L111" r:id="rId458" display="https://doi.org/10.48550/arXiv.1909.12555"/>
+    <hyperlink ref="R111" r:id="rId459" display="https://openreview.net/forum?id=8jmIpypMzE"/>
+    <hyperlink ref="G112" r:id="rId460" display="https://zenodo.org/record/4835278/files/article.pdf"/>
+    <hyperlink ref="H112" r:id="rId461" display="https://github.com/CampusAI/Hamiltonian-Generative-Networks"/>
+    <hyperlink ref="I112" r:id="rId462" display="https://openreview.net/forum?id=w23q3ttruo&amp;noteId=XenPH-P3an"/>
+    <hyperlink ref="L112" r:id="rId463" display="https://doi.org/10.48550/arXiv.1909.13789"/>
+    <hyperlink ref="R112" r:id="rId464" display="https://openreview.net/forum?id=Zszk4rXgesL"/>
+    <hyperlink ref="G113" r:id="rId465" display="https://zenodo.org/record/4835356/files/article.pdf"/>
+    <hyperlink ref="H113" r:id="rId466" display="https://github.com/maja601/pytorch-psetae"/>
+    <hyperlink ref="I113" r:id="rId467" display="https://ieeexplore.ieee.org/document/9157055"/>
+    <hyperlink ref="G114" r:id="rId468" display="https://zenodo.org/record/4835431/files/article.pdf"/>
+    <hyperlink ref="H114" r:id="rId469" display="https://github.com/GANA-FACT-AI/gana-fact-ai"/>
+    <hyperlink ref="I114" r:id="rId470" display="https://openreview.net/forum?id=S1xFl64tDr"/>
+    <hyperlink ref="L114" r:id="rId471" display="https://doi.org/10.48550/arXiv.1901.09546"/>
+    <hyperlink ref="R114" r:id="rId472" display="https://openreview.net/forum?id=P30M7d9DyXw"/>
+    <hyperlink ref="G115" r:id="rId473" display="https://zenodo.org/record/4835564/files/article.pdf"/>
+    <hyperlink ref="H115" r:id="rId474" display="https://github.com/varun19299/rigl-reproducibility"/>
+    <hyperlink ref="I115" r:id="rId475" display="https://openreview.net/forum?id=NqEF-9d38i6&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L115" r:id="rId476" display="https://doi.org/10.48550/arXiv.1911.11134"/>
+    <hyperlink ref="R115" r:id="rId477" display="https://openreview.net/forum?id=riCIeP6LzEE"/>
+    <hyperlink ref="G116" r:id="rId478" display="https://zenodo.org/record/4835592/files/article.pdf"/>
+    <hyperlink ref="H116" r:id="rId479" display="https://github.com/MotherOfUnicorns/FACT_AI_project"/>
+    <hyperlink ref="I116" r:id="rId480" display="https://openreview.net/forum?id=ykG2B9bWiPXe&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L116" r:id="rId481" display="https://doi.org/10.48550/arXiv.2004.14243"/>
+    <hyperlink ref="R116" r:id="rId482" display="https://openreview.net/forum?id=lE0wqKGROKa"/>
+    <hyperlink ref="G117" r:id="rId483" display="https://zenodo.org/record/4835600/files/article.pdf"/>
+    <hyperlink ref="H117" r:id="rId484" display="https://github.com/shin-ee-chen/UvA_FACT_2021"/>
+    <hyperlink ref="I117" r:id="rId485" display="https://openreview.net/forum?id=tdG6Fa3Y6hq&amp;referrer=%5BML%20Reproducibility%20Challenge%202020%5D(%2Fgroup%3Fid%3DML_Reproducibility_Challenge%2F2020)"/>
+    <hyperlink ref="L117" r:id="rId486" display="https://doi.org/10.48550/arXiv.2006.13913"/>
+    <hyperlink ref="R117" r:id="rId487" display="https://openreview.net/forum?id=Vqtf4kZg2j"/>
+    <hyperlink ref="G118" r:id="rId488" display="https://zenodo.org/record/4833117/files/article.pdf"/>
+    <hyperlink ref="G119" r:id="rId489" display="https://zenodo.org/record/3818627/files/article.pdf"/>
+    <hyperlink ref="G120" r:id="rId490" display="https://zenodo.org/record/3818607/files/article.pdf"/>
+    <hyperlink ref="H120" r:id="rId491" display="https://github.com/nancy-nayak/rethinking-bnn"/>
+    <hyperlink ref="I120" r:id="rId492" display="https://arxiv.org/abs/1906.02107"/>
+    <hyperlink ref="L120" r:id="rId493" display="https://doi.org/10.48550/arXiv.1906.02107"/>
+    <hyperlink ref="R120" r:id="rId494" display="https://openreview.net/forum?id=y53aaSM5o"/>
+    <hyperlink ref="G121" r:id="rId495" display="https://zenodo.org/record/3818609/files/article.pdf"/>
+    <hyperlink ref="H121" r:id="rId496" display="https://github.com/Xemnas0/NCSN-TF2.0"/>
+    <hyperlink ref="I121" r:id="rId497" display="https://arxiv.org/abs/1907.05600"/>
+    <hyperlink ref="L121" r:id="rId498" display="https://doi.org/10.48550/arXiv.1907.05600"/>
+    <hyperlink ref="R121" r:id="rId499" display="https://openreview.net/forum?id=B1lcYrBgLH"/>
+    <hyperlink ref="G122" r:id="rId500" display="https://zenodo.org/record/3818613/files/article.pdf"/>
+    <hyperlink ref="H122" r:id="rId501" display="https://github.com/lilfelix/reproducibility_NeurIPS19"/>
+    <hyperlink ref="I122" r:id="rId502" display="https://arxiv.org/abs/1901.10738"/>
+    <hyperlink ref="L122" r:id="rId503" display="https://doi.org/10.48550/arXiv.1901.10738"/>
+    <hyperlink ref="R122" r:id="rId504" display="https://openreview.net/forum?id=HyxQr65z6S"/>
+    <hyperlink ref="G123" r:id="rId505" display="https://zenodo.org/record/3818617/files/article.pdf"/>
+    <hyperlink ref="H123" r:id="rId506" display="https://github.com/LinuNils/TMC\_reproduced"/>
+    <hyperlink ref="I123" r:id="rId507" display="https://arxiv.org/abs/1806.08593"/>
+    <hyperlink ref="L123" r:id="rId508" display="https://doi.org/10.48550/arXiv.1806.08593"/>
+    <hyperlink ref="R123" r:id="rId509" display="https://openreview.net/forum?id=BJxUSaczTH"/>
+    <hyperlink ref="G124" r:id="rId510" display="https://zenodo.org/record/3818621/files/article.pdf"/>
+    <hyperlink ref="H124" r:id="rId511" display="https://github.com/ayushgarg31/HNN-Neurips2019"/>
+    <hyperlink ref="I124" r:id="rId512" display="https://arxiv.org/abs/1906.01563"/>
+    <hyperlink ref="L124" r:id="rId513" display="https://doi.org/10.48550/arXiv.1906.01563"/>
+    <hyperlink ref="R124" r:id="rId514" display="https://openreview.net/forum?id=HJxNSp9MTr"/>
+    <hyperlink ref="G125" r:id="rId515" display="https://zenodo.org/record/3818623/files/article.pdf"/>
+    <hyperlink ref="H125" r:id="rId516" display="https://github.com/AlexandrosFerles/NIPS_2019_Reproducibilty_Challenge_Zero-shot_Knowledge_Transfer_via_Adversarial_Belief_Matching"/>
+    <hyperlink ref="I125" r:id="rId517" display="https://arxiv.org/abs/1905.09768"/>
+    <hyperlink ref="L125" r:id="rId518" display="https://doi.org/10.48550/arXiv.1905.09768"/>
+    <hyperlink ref="G126" r:id="rId519" display="https://zenodo.org/record/3818611/files/article.pdf"/>
+    <hyperlink ref="H126" r:id="rId520" display="https://github.com/jxu43/replication-mbpo"/>
+    <hyperlink ref="I126" r:id="rId521" display="https://arxiv.org/abs/1906.08253"/>
+    <hyperlink ref="L126" r:id="rId522" display="https://doi.org/10.48550/arXiv.1906.08253"/>
+    <hyperlink ref="R126" r:id="rId523" display="https://openreview.net/forum?id=rkezvT9f6r"/>
+    <hyperlink ref="G127" r:id="rId524" display="https://zenodo.org/record/3818625/files/article.pdf"/>
+    <hyperlink ref="H127" r:id="rId525" display="https://github.com/GabrielAlacchi/atari-ari-extensions"/>
+    <hyperlink ref="I127" r:id="rId526" display="https://arxiv.org/abs/1906.08226"/>
+    <hyperlink ref="L127" r:id="rId527" display="https://doi.org/10.48550/arXiv.1906.08226"/>
+    <hyperlink ref="R127" r:id="rId528" display="https://openreview.net/forum?id=GAY8Xw9Qzs"/>
+    <hyperlink ref="G128" r:id="rId529" display="https://zenodo.org/record/3818619/files/article.pdf"/>
+    <hyperlink ref="H128" r:id="rId530" display="https://github.com/varungohil/Generalizing-Lottery-Tickets"/>
+    <hyperlink ref="I128" r:id="rId531" display="https://arxiv.org/abs/1906.02773"/>
+    <hyperlink ref="L128" r:id="rId532" display="https://doi.org/10.48550/arXiv.1906.02773"/>
+    <hyperlink ref="R128" r:id="rId533" display="https://openreview.net/forum?id=SklFHaqG6S"/>
+    <hyperlink ref="G129" r:id="rId534" display="https://zenodo.org/record/3818605/files/article.pdf"/>
+    <hyperlink ref="H129" r:id="rId535" display="https://github.com/MacroMayhem/OnMixup"/>
+    <hyperlink ref="I129" r:id="rId536" display="https://arxiv.org/abs/1905.11001"/>
+    <hyperlink ref="L129" r:id="rId537" display="https://doi.org/10.48550/arXiv.1905.11001"/>
+    <hyperlink ref="R129" r:id="rId538" display="https://openreview.net/forum?id=JhZOkalsiI"/>
+    <hyperlink ref="G130" r:id="rId539" display="https://zenodo.org/record/3158244/files/article.pdf"/>
+    <hyperlink ref="R130" r:id="rId540" display="https://github.com/ReScience/submissions/issues/5"/>
+    <hyperlink ref="G131" r:id="rId541" display="https://zenodo.org/record/3160540/files/article.pdf"/>
+    <hyperlink ref="H131" r:id="rId542" display="https://github.com/ArnoutDevos/r2d2"/>
+    <hyperlink ref="I131" r:id="rId543" display="https://arxiv.org/abs/1805.08136"/>
+    <hyperlink ref="L131" r:id="rId544" display="https://doi.org/10.48550/arXiv.1805.08136"/>
+    <hyperlink ref="R131" r:id="rId545" display="https://github.com/reproducibility-challenge/iclr_2019/pull/150"/>
+    <hyperlink ref="G132" r:id="rId546" display="https://zenodo.org/record/3161734/files/article.pdf"/>
+    <hyperlink ref="H132" r:id="rId547" display="https://github.com/Alfo5123/Variational-Sparse-Coding"/>
+    <hyperlink ref="I132" r:id="rId548" display="https://proceedings.mlr.press/v115/tonolini20a.html"/>
+    <hyperlink ref="R132" r:id="rId549" display="https://github.com/reproducibility-challenge/iclr_2019/pull/146"/>
+    <hyperlink ref="G133" r:id="rId550" display="https://zenodo.org/record/3162890/files/article.pdf"/>
+    <hyperlink ref="H133" r:id="rId551" display="https://github.com/francescobardi/pde_solver_deep_learned"/>
+    <hyperlink ref="I133" r:id="rId552" display="https://arxiv.org/abs/1906.01200"/>
+    <hyperlink ref="L133" r:id="rId553" display="https://doi.org/10.48550/arXiv.1906.01200"/>
+    <hyperlink ref="R133" r:id="rId554" display="https://github.com/reproducibility-challenge/iclr_2019/pull/136"/>
+    <hyperlink ref="G134" r:id="rId555" display="https://zenodo.org/record/3162114/files/article.pdf"/>
+    <hyperlink ref="H134" r:id="rId556" display="https://github.com/dido1998/h-detach/tree/v1.0"/>
+    <hyperlink ref="I134" r:id="rId557" display="https://arxiv.org/abs/1810.03023"/>
+    <hyperlink ref="L134" r:id="rId558" display="https://doi.org/10.48550/arXiv.1810.03023"/>
+    <hyperlink ref="R134" r:id="rId559" display="https://github.com/reproducibility-challenge/iclr_2019/pull/148"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId560"/>
+  <pageSetup orientation="portrait" paperSize="1" r:id="rId560"/>
 </worksheet>
 </file>
</xml_diff>